<commit_message>
R5 12 7 office
</commit_message>
<xml_diff>
--- a/inside_office/excel/準1級.xlsx
+++ b/inside_office/excel/準1級.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20404"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{481F39A4-C697-4788-9820-8A2741390EF7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A39EA00-FF06-4D65-A26E-64078C84D79C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10635" windowHeight="11445" firstSheet="13" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10635" windowHeight="11445" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="準1-1" sheetId="1" r:id="rId1"/>
@@ -3606,7 +3606,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3781,6 +3781,12 @@
     <xf numFmtId="40" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="40" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -28121,16 +28127,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19.5" thickBot="1">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="96" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94"/>
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
     </row>
     <row r="2" spans="1:11" ht="19.5" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -28157,10 +28163,10 @@
       <c r="H2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="95" t="s">
+      <c r="J2" s="97" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="95"/>
+      <c r="K2" s="97"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="5">
@@ -28343,19 +28349,19 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="19.5" thickBot="1">
-      <c r="A10" s="94" t="s">
+      <c r="A10" s="96" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="94"/>
-      <c r="C10" s="94"/>
-      <c r="D10" s="94"/>
-      <c r="E10" s="94"/>
-      <c r="F10" s="94"/>
-      <c r="G10" s="94"/>
-      <c r="H10" s="94"/>
-      <c r="I10" s="94"/>
-      <c r="J10" s="94"/>
-      <c r="K10" s="94"/>
+      <c r="B10" s="96"/>
+      <c r="C10" s="96"/>
+      <c r="D10" s="96"/>
+      <c r="E10" s="96"/>
+      <c r="F10" s="96"/>
+      <c r="G10" s="96"/>
+      <c r="H10" s="96"/>
+      <c r="I10" s="96"/>
+      <c r="J10" s="96"/>
+      <c r="K10" s="96"/>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="2" t="s">
@@ -28937,11 +28943,11 @@
       <c r="K25" s="10"/>
     </row>
     <row r="27" spans="1:11" ht="19.5" thickBot="1">
-      <c r="A27" s="95" t="s">
+      <c r="A27" s="97" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="95"/>
-      <c r="C27" s="95"/>
+      <c r="B27" s="97"/>
+      <c r="C27" s="97"/>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="2" t="s">
@@ -29053,22 +29059,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="96" t="s">
         <v>148</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="H1" s="95" t="s">
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="H1" s="97" t="s">
         <v>159</v>
       </c>
-      <c r="I1" s="95"/>
-      <c r="K1" s="95" t="s">
+      <c r="I1" s="97"/>
+      <c r="K1" s="97" t="s">
         <v>163</v>
       </c>
-      <c r="L1" s="95"/>
+      <c r="L1" s="97"/>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="2" t="s">
@@ -29233,20 +29239,20 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A8" s="94" t="s">
+      <c r="A8" s="96" t="s">
         <v>174</v>
       </c>
-      <c r="B8" s="94"/>
-      <c r="C8" s="94"/>
-      <c r="D8" s="94"/>
-      <c r="E8" s="94"/>
-      <c r="F8" s="94"/>
-      <c r="G8" s="94"/>
-      <c r="H8" s="94"/>
-      <c r="I8" s="94"/>
-      <c r="J8" s="94"/>
-      <c r="K8" s="94"/>
-      <c r="L8" s="94"/>
+      <c r="B8" s="96"/>
+      <c r="C8" s="96"/>
+      <c r="D8" s="96"/>
+      <c r="E8" s="96"/>
+      <c r="F8" s="96"/>
+      <c r="G8" s="96"/>
+      <c r="H8" s="96"/>
+      <c r="I8" s="96"/>
+      <c r="J8" s="96"/>
+      <c r="K8" s="96"/>
+      <c r="L8" s="96"/>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="2" t="s">
@@ -29921,11 +29927,11 @@
       <c r="L24" s="10"/>
     </row>
     <row r="26" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A26" s="107" t="s">
+      <c r="A26" s="109" t="s">
         <v>181</v>
       </c>
-      <c r="B26" s="107"/>
-      <c r="C26" s="107"/>
+      <c r="B26" s="109"/>
+      <c r="C26" s="109"/>
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="55" t="s">
@@ -30054,16 +30060,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="19.5" thickBot="1">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="96" t="s">
         <v>183</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94"/>
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
     </row>
     <row r="2" spans="1:14" ht="19.5" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -30090,14 +30096,14 @@
       <c r="H2" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="J2" s="95" t="s">
+      <c r="J2" s="97" t="s">
         <v>202</v>
       </c>
-      <c r="K2" s="95"/>
-      <c r="M2" s="94" t="s">
+      <c r="K2" s="97"/>
+      <c r="M2" s="96" t="s">
         <v>158</v>
       </c>
-      <c r="N2" s="94"/>
+      <c r="N2" s="96"/>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="5">
@@ -30354,10 +30360,10 @@
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
-      <c r="M9" s="94" t="s">
+      <c r="M9" s="96" t="s">
         <v>224</v>
       </c>
-      <c r="N9" s="94"/>
+      <c r="N9" s="96"/>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="5">
@@ -30420,10 +30426,10 @@
         <f t="shared" si="1"/>
         <v>63</v>
       </c>
-      <c r="J11" s="95" t="s">
+      <c r="J11" s="97" t="s">
         <v>208</v>
       </c>
-      <c r="K11" s="95"/>
+      <c r="K11" s="97"/>
       <c r="M11" s="5">
         <v>1</v>
       </c>
@@ -30490,20 +30496,20 @@
       </c>
     </row>
     <row r="15" spans="1:14" ht="19.5" thickBot="1">
-      <c r="A15" s="106" t="s">
+      <c r="A15" s="108" t="s">
         <v>211</v>
       </c>
-      <c r="B15" s="106"/>
-      <c r="C15" s="106"/>
-      <c r="D15" s="106"/>
-      <c r="E15" s="106"/>
-      <c r="F15" s="106"/>
-      <c r="G15" s="106"/>
-      <c r="H15" s="106"/>
-      <c r="I15" s="106"/>
-      <c r="J15" s="106"/>
-      <c r="K15" s="106"/>
-      <c r="L15" s="106"/>
+      <c r="B15" s="108"/>
+      <c r="C15" s="108"/>
+      <c r="D15" s="108"/>
+      <c r="E15" s="108"/>
+      <c r="F15" s="108"/>
+      <c r="G15" s="108"/>
+      <c r="H15" s="108"/>
+      <c r="I15" s="108"/>
+      <c r="J15" s="108"/>
+      <c r="K15" s="108"/>
+      <c r="L15" s="108"/>
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="2" t="s">
@@ -31013,12 +31019,12 @@
     </row>
     <row r="29" spans="1:12" ht="19.5" thickBot="1"/>
     <row r="30" spans="1:12">
-      <c r="A30" s="102" t="s">
+      <c r="A30" s="104" t="s">
         <v>225</v>
       </c>
-      <c r="B30" s="103"/>
-      <c r="C30" s="103"/>
-      <c r="D30" s="103"/>
+      <c r="B30" s="105"/>
+      <c r="C30" s="105"/>
+      <c r="D30" s="105"/>
       <c r="E30" s="69">
         <f>ROUND(DAVERAGE(総支給額一覧表6,K16,$I$30:$I$31),0)</f>
         <v>327735</v>
@@ -31031,12 +31037,12 @@
       </c>
     </row>
     <row r="31" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A31" s="104" t="s">
+      <c r="A31" s="106" t="s">
         <v>226</v>
       </c>
-      <c r="B31" s="105"/>
-      <c r="C31" s="105"/>
-      <c r="D31" s="105"/>
+      <c r="B31" s="107"/>
+      <c r="C31" s="107"/>
+      <c r="D31" s="107"/>
       <c r="E31" s="14">
         <f>DSUM(総支給額一覧表6,G16,$K$30:$K$31)</f>
         <v>68815</v>
@@ -31099,16 +31105,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="19.5" thickBot="1">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="96" t="s">
         <v>183</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94"/>
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
     </row>
     <row r="2" spans="1:14" ht="19.5" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -31135,14 +31141,14 @@
       <c r="H2" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="J2" s="95" t="s">
+      <c r="J2" s="97" t="s">
         <v>202</v>
       </c>
-      <c r="K2" s="95"/>
-      <c r="M2" s="94" t="s">
+      <c r="K2" s="97"/>
+      <c r="M2" s="96" t="s">
         <v>134</v>
       </c>
-      <c r="N2" s="94"/>
+      <c r="N2" s="96"/>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="5">
@@ -31399,10 +31405,10 @@
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
-      <c r="M9" s="94" t="s">
+      <c r="M9" s="96" t="s">
         <v>224</v>
       </c>
-      <c r="N9" s="94"/>
+      <c r="N9" s="96"/>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="5">
@@ -31465,10 +31471,10 @@
         <f t="shared" si="1"/>
         <v>63</v>
       </c>
-      <c r="J11" s="95" t="s">
+      <c r="J11" s="97" t="s">
         <v>208</v>
       </c>
-      <c r="K11" s="95"/>
+      <c r="K11" s="97"/>
       <c r="M11" s="5">
         <v>1</v>
       </c>
@@ -31535,20 +31541,20 @@
       </c>
     </row>
     <row r="15" spans="1:14" ht="19.5" thickBot="1">
-      <c r="A15" s="106" t="s">
+      <c r="A15" s="108" t="s">
         <v>211</v>
       </c>
-      <c r="B15" s="106"/>
-      <c r="C15" s="106"/>
-      <c r="D15" s="106"/>
-      <c r="E15" s="106"/>
-      <c r="F15" s="106"/>
-      <c r="G15" s="106"/>
-      <c r="H15" s="106"/>
-      <c r="I15" s="106"/>
-      <c r="J15" s="106"/>
-      <c r="K15" s="106"/>
-      <c r="L15" s="106"/>
+      <c r="B15" s="108"/>
+      <c r="C15" s="108"/>
+      <c r="D15" s="108"/>
+      <c r="E15" s="108"/>
+      <c r="F15" s="108"/>
+      <c r="G15" s="108"/>
+      <c r="H15" s="108"/>
+      <c r="I15" s="108"/>
+      <c r="J15" s="108"/>
+      <c r="K15" s="108"/>
+      <c r="L15" s="108"/>
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="2" t="s">
@@ -32058,12 +32064,12 @@
     </row>
     <row r="29" spans="1:12" ht="19.5" thickBot="1"/>
     <row r="30" spans="1:12">
-      <c r="A30" s="102" t="s">
+      <c r="A30" s="104" t="s">
         <v>225</v>
       </c>
-      <c r="B30" s="103"/>
-      <c r="C30" s="103"/>
-      <c r="D30" s="103"/>
+      <c r="B30" s="105"/>
+      <c r="C30" s="105"/>
+      <c r="D30" s="105"/>
       <c r="E30" s="69">
         <f>ROUND(DAVERAGE(総支給額一覧表6,K16,$I$30:$I$31),0)</f>
         <v>327735</v>
@@ -32076,12 +32082,12 @@
       </c>
     </row>
     <row r="31" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A31" s="104" t="s">
+      <c r="A31" s="106" t="s">
         <v>226</v>
       </c>
-      <c r="B31" s="105"/>
-      <c r="C31" s="105"/>
-      <c r="D31" s="105"/>
+      <c r="B31" s="107"/>
+      <c r="C31" s="107"/>
+      <c r="D31" s="107"/>
       <c r="E31" s="14">
         <f>DSUM(総支給額一覧表6,G16,$K$30:$K$31)</f>
         <v>68815</v>
@@ -32132,16 +32138,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" thickBot="1">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="96" t="s">
         <v>229</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94"/>
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
@@ -32327,17 +32333,17 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="19.5" thickBot="1">
-      <c r="A10" s="94" t="s">
+      <c r="A10" s="96" t="s">
         <v>246</v>
       </c>
-      <c r="B10" s="94"/>
-      <c r="C10" s="94"/>
-      <c r="D10" s="94"/>
-      <c r="E10" s="94"/>
-      <c r="F10" s="94"/>
-      <c r="G10" s="94"/>
-      <c r="H10" s="94"/>
-      <c r="I10" s="94"/>
+      <c r="B10" s="96"/>
+      <c r="C10" s="96"/>
+      <c r="D10" s="96"/>
+      <c r="E10" s="96"/>
+      <c r="F10" s="96"/>
+      <c r="G10" s="96"/>
+      <c r="H10" s="96"/>
+      <c r="I10" s="96"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="2" t="s">
@@ -32688,18 +32694,18 @@
       <c r="I21" s="10"/>
     </row>
     <row r="23" spans="1:9" ht="19.5" thickBot="1">
-      <c r="A23" s="94" t="s">
+      <c r="A23" s="96" t="s">
         <v>247</v>
       </c>
-      <c r="B23" s="94"/>
-      <c r="C23" s="94"/>
-      <c r="D23" s="94"/>
+      <c r="B23" s="96"/>
+      <c r="C23" s="96"/>
+      <c r="D23" s="96"/>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="110" t="s">
+      <c r="A24" s="112" t="s">
         <v>231</v>
       </c>
-      <c r="B24" s="111"/>
+      <c r="B24" s="113"/>
       <c r="C24" s="3" t="s">
         <v>244</v>
       </c>
@@ -32720,10 +32726,10 @@
       </c>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="108" t="s">
+      <c r="A25" s="110" t="s">
         <v>239</v>
       </c>
-      <c r="B25" s="109"/>
+      <c r="B25" s="111"/>
       <c r="C25" s="11">
         <f>DSUM(株式売却一覧表7,C$24,$F$24:$F$25)</f>
         <v>15429</v>
@@ -32746,10 +32752,10 @@
       </c>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26" s="108" t="s">
+      <c r="A26" s="110" t="s">
         <v>240</v>
       </c>
-      <c r="B26" s="109"/>
+      <c r="B26" s="111"/>
       <c r="C26" s="11">
         <f>DSUM(株式売却一覧表7,C$24,$G$24:$G$25)</f>
         <v>24961</v>
@@ -32760,10 +32766,10 @@
       </c>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="108" t="s">
+      <c r="A27" s="110" t="s">
         <v>241</v>
       </c>
-      <c r="B27" s="109"/>
+      <c r="B27" s="111"/>
       <c r="C27" s="11">
         <f>DSUM(株式売却一覧表7,C$24,$H$24:$H$25)</f>
         <v>19858</v>
@@ -32774,10 +32780,10 @@
       </c>
     </row>
     <row r="28" spans="1:9" ht="19.5" thickBot="1">
-      <c r="A28" s="104" t="s">
+      <c r="A28" s="106" t="s">
         <v>243</v>
       </c>
-      <c r="B28" s="105"/>
+      <c r="B28" s="107"/>
       <c r="C28" s="13">
         <f>DSUM(株式売却一覧表7,C$24,$I$24:$I$25)</f>
         <v>22820</v>
@@ -32833,16 +32839,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" thickBot="1">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="96" t="s">
         <v>229</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94"/>
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
@@ -33028,17 +33034,17 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="19.5" thickBot="1">
-      <c r="A10" s="94" t="s">
+      <c r="A10" s="96" t="s">
         <v>246</v>
       </c>
-      <c r="B10" s="94"/>
-      <c r="C10" s="94"/>
-      <c r="D10" s="94"/>
-      <c r="E10" s="94"/>
-      <c r="F10" s="94"/>
-      <c r="G10" s="94"/>
-      <c r="H10" s="94"/>
-      <c r="I10" s="94"/>
+      <c r="B10" s="96"/>
+      <c r="C10" s="96"/>
+      <c r="D10" s="96"/>
+      <c r="E10" s="96"/>
+      <c r="F10" s="96"/>
+      <c r="G10" s="96"/>
+      <c r="H10" s="96"/>
+      <c r="I10" s="96"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="2" t="s">
@@ -33389,18 +33395,18 @@
       <c r="I21" s="10"/>
     </row>
     <row r="23" spans="1:9" ht="19.5" thickBot="1">
-      <c r="A23" s="94" t="s">
+      <c r="A23" s="96" t="s">
         <v>247</v>
       </c>
-      <c r="B23" s="94"/>
-      <c r="C23" s="94"/>
-      <c r="D23" s="94"/>
+      <c r="B23" s="96"/>
+      <c r="C23" s="96"/>
+      <c r="D23" s="96"/>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="110" t="s">
+      <c r="A24" s="112" t="s">
         <v>231</v>
       </c>
-      <c r="B24" s="111"/>
+      <c r="B24" s="113"/>
       <c r="C24" s="3" t="s">
         <v>244</v>
       </c>
@@ -33421,10 +33427,10 @@
       </c>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="108" t="s">
+      <c r="A25" s="110" t="s">
         <v>239</v>
       </c>
-      <c r="B25" s="109"/>
+      <c r="B25" s="111"/>
       <c r="C25" s="11">
         <f>DSUM(株式売却一覧表7,C$24,$F$24:$F$25)</f>
         <v>15429</v>
@@ -33447,10 +33453,10 @@
       </c>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26" s="108" t="s">
+      <c r="A26" s="110" t="s">
         <v>240</v>
       </c>
-      <c r="B26" s="109"/>
+      <c r="B26" s="111"/>
       <c r="C26" s="11">
         <f>DSUM(株式売却一覧表7,C$24,$G$24:$G$25)</f>
         <v>24961</v>
@@ -33461,10 +33467,10 @@
       </c>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="108" t="s">
+      <c r="A27" s="110" t="s">
         <v>241</v>
       </c>
-      <c r="B27" s="109"/>
+      <c r="B27" s="111"/>
       <c r="C27" s="11">
         <f>DSUM(株式売却一覧表7,C$24,$H$24:$H$25)</f>
         <v>19858</v>
@@ -33475,10 +33481,10 @@
       </c>
     </row>
     <row r="28" spans="1:9" ht="19.5" thickBot="1">
-      <c r="A28" s="104" t="s">
+      <c r="A28" s="106" t="s">
         <v>243</v>
       </c>
-      <c r="B28" s="105"/>
+      <c r="B28" s="107"/>
       <c r="C28" s="13">
         <f>DSUM(株式売却一覧表7,C$24,$I$24:$I$25)</f>
         <v>22820</v>
@@ -33533,22 +33539,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19.5" thickBot="1">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="96" t="s">
         <v>250</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94"/>
-      <c r="I1" s="94"/>
-      <c r="K1" s="94" t="s">
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="96"/>
+      <c r="K1" s="96" t="s">
         <v>262</v>
       </c>
-      <c r="L1" s="94"/>
-      <c r="M1" s="94"/>
+      <c r="L1" s="96"/>
+      <c r="M1" s="96"/>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="2" t="s">
@@ -33931,22 +33937,22 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="19.5" thickBot="1">
-      <c r="A14" s="94" t="s">
+      <c r="A14" s="96" t="s">
         <v>267</v>
       </c>
-      <c r="B14" s="94"/>
-      <c r="C14" s="94"/>
-      <c r="D14" s="94"/>
-      <c r="E14" s="94"/>
-      <c r="F14" s="94"/>
-      <c r="G14" s="94"/>
-      <c r="H14" s="94"/>
-      <c r="I14" s="94"/>
-      <c r="J14" s="94"/>
-      <c r="L14" s="94" t="s">
+      <c r="B14" s="96"/>
+      <c r="C14" s="96"/>
+      <c r="D14" s="96"/>
+      <c r="E14" s="96"/>
+      <c r="F14" s="96"/>
+      <c r="G14" s="96"/>
+      <c r="H14" s="96"/>
+      <c r="I14" s="96"/>
+      <c r="J14" s="96"/>
+      <c r="L14" s="96" t="s">
         <v>271</v>
       </c>
-      <c r="M14" s="94"/>
+      <c r="M14" s="96"/>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="2" t="s">
@@ -34410,12 +34416,12 @@
     </row>
     <row r="28" spans="1:13" ht="19.5" thickBot="1"/>
     <row r="29" spans="1:13">
-      <c r="A29" s="102" t="s">
+      <c r="A29" s="104" t="s">
         <v>272</v>
       </c>
-      <c r="B29" s="103"/>
-      <c r="C29" s="103"/>
-      <c r="D29" s="103"/>
+      <c r="B29" s="105"/>
+      <c r="C29" s="105"/>
+      <c r="D29" s="105"/>
       <c r="E29" s="18">
         <f>DCOUNT(請求額一覧表8, E15, G29:G30)</f>
         <v>3</v>
@@ -34428,12 +34434,12 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="19.5" thickBot="1">
-      <c r="A30" s="104" t="s">
+      <c r="A30" s="106" t="s">
         <v>273</v>
       </c>
-      <c r="B30" s="105"/>
-      <c r="C30" s="105"/>
-      <c r="D30" s="105"/>
+      <c r="B30" s="107"/>
+      <c r="C30" s="107"/>
+      <c r="D30" s="107"/>
       <c r="E30" s="14">
         <f>ROUND(DAVERAGE(請求額一覧表8,H15, I29:I30),0)</f>
         <v>509766</v>
@@ -34472,7 +34478,7 @@
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView showFormulas="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:M1048576"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -34492,22 +34498,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19.5" thickBot="1">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="96" t="s">
         <v>250</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94"/>
-      <c r="I1" s="94"/>
-      <c r="K1" s="94" t="s">
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="96"/>
+      <c r="K1" s="96" t="s">
         <v>262</v>
       </c>
-      <c r="L1" s="94"/>
-      <c r="M1" s="94"/>
+      <c r="L1" s="96"/>
+      <c r="M1" s="96"/>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="2" t="s">
@@ -34890,22 +34896,22 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="19.5" thickBot="1">
-      <c r="A14" s="94" t="s">
+      <c r="A14" s="96" t="s">
         <v>267</v>
       </c>
-      <c r="B14" s="94"/>
-      <c r="C14" s="94"/>
-      <c r="D14" s="94"/>
-      <c r="E14" s="94"/>
-      <c r="F14" s="94"/>
-      <c r="G14" s="94"/>
-      <c r="H14" s="94"/>
-      <c r="I14" s="94"/>
-      <c r="J14" s="94"/>
-      <c r="L14" s="94" t="s">
+      <c r="B14" s="96"/>
+      <c r="C14" s="96"/>
+      <c r="D14" s="96"/>
+      <c r="E14" s="96"/>
+      <c r="F14" s="96"/>
+      <c r="G14" s="96"/>
+      <c r="H14" s="96"/>
+      <c r="I14" s="96"/>
+      <c r="J14" s="96"/>
+      <c r="L14" s="96" t="s">
         <v>271</v>
       </c>
-      <c r="M14" s="94"/>
+      <c r="M14" s="96"/>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="2" t="s">
@@ -35369,12 +35375,12 @@
     </row>
     <row r="28" spans="1:13" ht="19.5" thickBot="1"/>
     <row r="29" spans="1:13">
-      <c r="A29" s="102" t="s">
+      <c r="A29" s="104" t="s">
         <v>272</v>
       </c>
-      <c r="B29" s="103"/>
-      <c r="C29" s="103"/>
-      <c r="D29" s="103"/>
+      <c r="B29" s="105"/>
+      <c r="C29" s="105"/>
+      <c r="D29" s="105"/>
       <c r="E29" s="18">
         <f>DCOUNT(請求額一覧表8, E15, G29:G30)</f>
         <v>3</v>
@@ -35387,12 +35393,12 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="19.5" thickBot="1">
-      <c r="A30" s="104" t="s">
+      <c r="A30" s="106" t="s">
         <v>273</v>
       </c>
-      <c r="B30" s="105"/>
-      <c r="C30" s="105"/>
-      <c r="D30" s="105"/>
+      <c r="B30" s="107"/>
+      <c r="C30" s="107"/>
+      <c r="D30" s="107"/>
       <c r="E30" s="14">
         <f>ROUND(DAVERAGE(請求額一覧表8,H15, I29:I30),0)</f>
         <v>509766</v>
@@ -35443,22 +35449,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19.5" thickBot="1">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="96" t="s">
         <v>278</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94"/>
-      <c r="J1" s="94" t="s">
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="J1" s="96" t="s">
         <v>300</v>
       </c>
-      <c r="K1" s="94"/>
-      <c r="L1" s="94"/>
-      <c r="M1" s="94"/>
+      <c r="K1" s="96"/>
+      <c r="L1" s="96"/>
+      <c r="M1" s="96"/>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="2" t="s">
@@ -35818,21 +35824,21 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="19.5" thickBot="1">
-      <c r="A14" s="94" t="s">
+      <c r="A14" s="96" t="s">
         <v>283</v>
       </c>
-      <c r="B14" s="94"/>
-      <c r="C14" s="94"/>
-      <c r="D14" s="94"/>
-      <c r="E14" s="94"/>
-      <c r="F14" s="94"/>
-      <c r="G14" s="94"/>
-      <c r="H14" s="94"/>
-      <c r="I14" s="94"/>
-      <c r="K14" s="94" t="s">
+      <c r="B14" s="96"/>
+      <c r="C14" s="96"/>
+      <c r="D14" s="96"/>
+      <c r="E14" s="96"/>
+      <c r="F14" s="96"/>
+      <c r="G14" s="96"/>
+      <c r="H14" s="96"/>
+      <c r="I14" s="96"/>
+      <c r="K14" s="96" t="s">
         <v>271</v>
       </c>
-      <c r="L14" s="94"/>
+      <c r="L14" s="96"/>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="2" t="s">
@@ -36216,12 +36222,12 @@
     </row>
     <row r="27" spans="1:12" ht="19.5" thickBot="1"/>
     <row r="28" spans="1:12">
-      <c r="A28" s="102" t="s">
+      <c r="A28" s="104" t="s">
         <v>301</v>
       </c>
-      <c r="B28" s="103"/>
-      <c r="C28" s="103"/>
-      <c r="D28" s="103"/>
+      <c r="B28" s="105"/>
+      <c r="C28" s="105"/>
+      <c r="D28" s="105"/>
       <c r="E28" s="18">
         <f>DCOUNT(請求金額一覧表9,C15,G28:G29)</f>
         <v>4</v>
@@ -36234,12 +36240,12 @@
       </c>
     </row>
     <row r="29" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A29" s="104" t="s">
+      <c r="A29" s="106" t="s">
         <v>302</v>
       </c>
-      <c r="B29" s="105"/>
-      <c r="C29" s="105"/>
-      <c r="D29" s="105"/>
+      <c r="B29" s="107"/>
+      <c r="C29" s="107"/>
+      <c r="D29" s="107"/>
       <c r="E29" s="14">
         <f>DSUM(請求金額一覧表9,H15,I28:I29)</f>
         <v>122993</v>
@@ -36297,22 +36303,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19.5" thickBot="1">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="96" t="s">
         <v>278</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94"/>
-      <c r="J1" s="94" t="s">
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="J1" s="96" t="s">
         <v>300</v>
       </c>
-      <c r="K1" s="94"/>
-      <c r="L1" s="94"/>
-      <c r="M1" s="94"/>
+      <c r="K1" s="96"/>
+      <c r="L1" s="96"/>
+      <c r="M1" s="96"/>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="2" t="s">
@@ -36672,21 +36678,21 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="19.5" thickBot="1">
-      <c r="A14" s="94" t="s">
+      <c r="A14" s="96" t="s">
         <v>283</v>
       </c>
-      <c r="B14" s="94"/>
-      <c r="C14" s="94"/>
-      <c r="D14" s="94"/>
-      <c r="E14" s="94"/>
-      <c r="F14" s="94"/>
-      <c r="G14" s="94"/>
-      <c r="H14" s="94"/>
-      <c r="I14" s="94"/>
-      <c r="K14" s="94" t="s">
+      <c r="B14" s="96"/>
+      <c r="C14" s="96"/>
+      <c r="D14" s="96"/>
+      <c r="E14" s="96"/>
+      <c r="F14" s="96"/>
+      <c r="G14" s="96"/>
+      <c r="H14" s="96"/>
+      <c r="I14" s="96"/>
+      <c r="K14" s="96" t="s">
         <v>271</v>
       </c>
-      <c r="L14" s="94"/>
+      <c r="L14" s="96"/>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="2" t="s">
@@ -37070,12 +37076,12 @@
     </row>
     <row r="27" spans="1:12" ht="19.5" thickBot="1"/>
     <row r="28" spans="1:12">
-      <c r="A28" s="102" t="s">
+      <c r="A28" s="104" t="s">
         <v>301</v>
       </c>
-      <c r="B28" s="103"/>
-      <c r="C28" s="103"/>
-      <c r="D28" s="103"/>
+      <c r="B28" s="105"/>
+      <c r="C28" s="105"/>
+      <c r="D28" s="105"/>
       <c r="E28" s="18">
         <f>DCOUNT(請求金額一覧表9,C15,G28:G29)</f>
         <v>4</v>
@@ -37088,12 +37094,12 @@
       </c>
     </row>
     <row r="29" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A29" s="104" t="s">
+      <c r="A29" s="106" t="s">
         <v>302</v>
       </c>
-      <c r="B29" s="105"/>
-      <c r="C29" s="105"/>
-      <c r="D29" s="105"/>
+      <c r="B29" s="107"/>
+      <c r="C29" s="107"/>
+      <c r="D29" s="107"/>
       <c r="E29" s="14">
         <f>DSUM(請求金額一覧表9,H15,I28:I29)</f>
         <v>122993</v>
@@ -37144,23 +37150,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19.5" thickBot="1">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="108" t="s">
         <v>307</v>
       </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
-      <c r="G1" s="106"/>
-      <c r="H1" s="106"/>
-      <c r="I1" s="106"/>
+      <c r="B1" s="108"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
+      <c r="G1" s="108"/>
+      <c r="H1" s="108"/>
+      <c r="I1" s="108"/>
       <c r="J1" s="84"/>
-      <c r="K1" s="95" t="s">
+      <c r="K1" s="97" t="s">
         <v>321</v>
       </c>
-      <c r="L1" s="95"/>
-      <c r="M1" s="95"/>
+      <c r="L1" s="97"/>
+      <c r="M1" s="97"/>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="81" t="s">
@@ -37536,21 +37542,21 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="19.5" thickBot="1">
-      <c r="A14" s="94" t="s">
+      <c r="A14" s="96" t="s">
         <v>267</v>
       </c>
-      <c r="B14" s="94"/>
-      <c r="C14" s="94"/>
-      <c r="D14" s="94"/>
-      <c r="E14" s="94"/>
-      <c r="F14" s="94"/>
-      <c r="G14" s="94"/>
-      <c r="H14" s="94"/>
-      <c r="I14" s="94"/>
-      <c r="K14" s="94" t="s">
+      <c r="B14" s="96"/>
+      <c r="C14" s="96"/>
+      <c r="D14" s="96"/>
+      <c r="E14" s="96"/>
+      <c r="F14" s="96"/>
+      <c r="G14" s="96"/>
+      <c r="H14" s="96"/>
+      <c r="I14" s="96"/>
+      <c r="K14" s="96" t="s">
         <v>337</v>
       </c>
-      <c r="L14" s="94"/>
+      <c r="L14" s="96"/>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="81" t="s">
@@ -37934,12 +37940,12 @@
     </row>
     <row r="27" spans="1:12" ht="19.5" thickBot="1"/>
     <row r="28" spans="1:12">
-      <c r="A28" s="102" t="s">
+      <c r="A28" s="104" t="s">
         <v>338</v>
       </c>
-      <c r="B28" s="103"/>
-      <c r="C28" s="103"/>
-      <c r="D28" s="103"/>
+      <c r="B28" s="105"/>
+      <c r="C28" s="105"/>
+      <c r="D28" s="105"/>
       <c r="E28" s="69">
         <f>DSUM(請求額一覧表10,E15,K28:K29)</f>
         <v>75279</v>
@@ -37952,12 +37958,12 @@
       </c>
     </row>
     <row r="29" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A29" s="104" t="s">
+      <c r="A29" s="106" t="s">
         <v>339</v>
       </c>
-      <c r="B29" s="105"/>
-      <c r="C29" s="105"/>
-      <c r="D29" s="105"/>
+      <c r="B29" s="107"/>
+      <c r="C29" s="107"/>
+      <c r="D29" s="107"/>
       <c r="E29" s="14">
         <f>DMAX(請求額一覧表10,H15,L28:L29)</f>
         <v>76655</v>
@@ -37996,7 +38002,7 @@
   <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView showFormulas="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -38013,16 +38019,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19.5" thickBot="1">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="96" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94"/>
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
     </row>
     <row r="2" spans="1:11" ht="19.5" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -38049,10 +38055,10 @@
       <c r="H2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="95" t="s">
+      <c r="J2" s="97" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="95"/>
+      <c r="K2" s="97"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="5">
@@ -38235,19 +38241,19 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="19.5" thickBot="1">
-      <c r="A10" s="94" t="s">
+      <c r="A10" s="96" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="94"/>
-      <c r="C10" s="94"/>
-      <c r="D10" s="94"/>
-      <c r="E10" s="94"/>
-      <c r="F10" s="94"/>
-      <c r="G10" s="94"/>
-      <c r="H10" s="94"/>
-      <c r="I10" s="94"/>
-      <c r="J10" s="94"/>
-      <c r="K10" s="94"/>
+      <c r="B10" s="96"/>
+      <c r="C10" s="96"/>
+      <c r="D10" s="96"/>
+      <c r="E10" s="96"/>
+      <c r="F10" s="96"/>
+      <c r="G10" s="96"/>
+      <c r="H10" s="96"/>
+      <c r="I10" s="96"/>
+      <c r="J10" s="96"/>
+      <c r="K10" s="96"/>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="2" t="s">
@@ -38829,11 +38835,11 @@
       <c r="K25" s="10"/>
     </row>
     <row r="27" spans="1:11" ht="19.5" thickBot="1">
-      <c r="A27" s="95" t="s">
+      <c r="A27" s="97" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="95"/>
-      <c r="C27" s="95"/>
+      <c r="B27" s="97"/>
+      <c r="C27" s="97"/>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="2" t="s">
@@ -38943,23 +38949,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19.5" thickBot="1">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="108" t="s">
         <v>307</v>
       </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
-      <c r="G1" s="106"/>
-      <c r="H1" s="106"/>
-      <c r="I1" s="106"/>
+      <c r="B1" s="108"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
+      <c r="G1" s="108"/>
+      <c r="H1" s="108"/>
+      <c r="I1" s="108"/>
       <c r="J1" s="84"/>
-      <c r="K1" s="95" t="s">
+      <c r="K1" s="97" t="s">
         <v>321</v>
       </c>
-      <c r="L1" s="95"/>
-      <c r="M1" s="95"/>
+      <c r="L1" s="97"/>
+      <c r="M1" s="97"/>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="81" t="s">
@@ -39335,21 +39341,21 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="19.5" thickBot="1">
-      <c r="A14" s="94" t="s">
+      <c r="A14" s="96" t="s">
         <v>267</v>
       </c>
-      <c r="B14" s="94"/>
-      <c r="C14" s="94"/>
-      <c r="D14" s="94"/>
-      <c r="E14" s="94"/>
-      <c r="F14" s="94"/>
-      <c r="G14" s="94"/>
-      <c r="H14" s="94"/>
-      <c r="I14" s="94"/>
-      <c r="K14" s="94" t="s">
+      <c r="B14" s="96"/>
+      <c r="C14" s="96"/>
+      <c r="D14" s="96"/>
+      <c r="E14" s="96"/>
+      <c r="F14" s="96"/>
+      <c r="G14" s="96"/>
+      <c r="H14" s="96"/>
+      <c r="I14" s="96"/>
+      <c r="K14" s="96" t="s">
         <v>337</v>
       </c>
-      <c r="L14" s="94"/>
+      <c r="L14" s="96"/>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="81" t="s">
@@ -39733,12 +39739,12 @@
     </row>
     <row r="27" spans="1:12" ht="19.5" thickBot="1"/>
     <row r="28" spans="1:12">
-      <c r="A28" s="102" t="s">
+      <c r="A28" s="104" t="s">
         <v>338</v>
       </c>
-      <c r="B28" s="103"/>
-      <c r="C28" s="103"/>
-      <c r="D28" s="103"/>
+      <c r="B28" s="105"/>
+      <c r="C28" s="105"/>
+      <c r="D28" s="105"/>
       <c r="E28" s="69">
         <f>DSUM(請求額一覧表10,E15,K28:K29)</f>
         <v>75279</v>
@@ -39751,12 +39757,12 @@
       </c>
     </row>
     <row r="29" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A29" s="104" t="s">
+      <c r="A29" s="106" t="s">
         <v>339</v>
       </c>
-      <c r="B29" s="105"/>
-      <c r="C29" s="105"/>
-      <c r="D29" s="105"/>
+      <c r="B29" s="107"/>
+      <c r="C29" s="107"/>
+      <c r="D29" s="107"/>
       <c r="E29" s="14">
         <f>DMAX(請求額一覧表10,H15,L28:L29)</f>
         <v>76655</v>
@@ -39810,15 +39816,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19.5" thickBot="1">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="108" t="s">
         <v>343</v>
       </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
-      <c r="G1" s="106"/>
+      <c r="B1" s="108"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
+      <c r="G1" s="108"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="81" t="s">
@@ -39948,19 +39954,19 @@
       <c r="G7" s="10"/>
     </row>
     <row r="9" spans="1:11" ht="19.5" thickBot="1">
-      <c r="A9" s="94" t="s">
+      <c r="A9" s="96" t="s">
         <v>355</v>
       </c>
-      <c r="B9" s="94"/>
-      <c r="C9" s="94"/>
-      <c r="D9" s="94"/>
-      <c r="E9" s="94"/>
-      <c r="F9" s="94"/>
-      <c r="G9" s="94"/>
-      <c r="H9" s="94"/>
-      <c r="I9" s="94"/>
-      <c r="J9" s="94"/>
-      <c r="K9" s="94"/>
+      <c r="B9" s="96"/>
+      <c r="C9" s="96"/>
+      <c r="D9" s="96"/>
+      <c r="E9" s="96"/>
+      <c r="F9" s="96"/>
+      <c r="G9" s="96"/>
+      <c r="H9" s="96"/>
+      <c r="I9" s="96"/>
+      <c r="J9" s="96"/>
+      <c r="K9" s="96"/>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="81" t="s">
@@ -40416,11 +40422,11 @@
       </c>
     </row>
     <row r="23" spans="1:11" ht="19.5" thickBot="1">
-      <c r="A23" s="94" t="s">
+      <c r="A23" s="96" t="s">
         <v>375</v>
       </c>
-      <c r="B23" s="94"/>
-      <c r="C23" s="94"/>
+      <c r="B23" s="96"/>
+      <c r="C23" s="96"/>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="81" t="s">
@@ -40513,8 +40519,8 @@
   </sheetPr>
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView showFormulas="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:K1048576"/>
+    <sheetView showFormulas="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -40533,15 +40539,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19.5" thickBot="1">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="108" t="s">
         <v>343</v>
       </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
-      <c r="G1" s="106"/>
+      <c r="B1" s="108"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
+      <c r="G1" s="108"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="81" t="s">
@@ -40671,19 +40677,19 @@
       <c r="G7" s="10"/>
     </row>
     <row r="9" spans="1:11" ht="19.5" thickBot="1">
-      <c r="A9" s="94" t="s">
+      <c r="A9" s="96" t="s">
         <v>355</v>
       </c>
-      <c r="B9" s="94"/>
-      <c r="C9" s="94"/>
-      <c r="D9" s="94"/>
-      <c r="E9" s="94"/>
-      <c r="F9" s="94"/>
-      <c r="G9" s="94"/>
-      <c r="H9" s="94"/>
-      <c r="I9" s="94"/>
-      <c r="J9" s="94"/>
-      <c r="K9" s="94"/>
+      <c r="B9" s="96"/>
+      <c r="C9" s="96"/>
+      <c r="D9" s="96"/>
+      <c r="E9" s="96"/>
+      <c r="F9" s="96"/>
+      <c r="G9" s="96"/>
+      <c r="H9" s="96"/>
+      <c r="I9" s="96"/>
+      <c r="J9" s="96"/>
+      <c r="K9" s="96"/>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="81" t="s">
@@ -41139,11 +41145,11 @@
       </c>
     </row>
     <row r="23" spans="1:11" ht="19.5" thickBot="1">
-      <c r="A23" s="94" t="s">
+      <c r="A23" s="96" t="s">
         <v>375</v>
       </c>
-      <c r="B23" s="94"/>
-      <c r="C23" s="94"/>
+      <c r="B23" s="96"/>
+      <c r="C23" s="96"/>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="81" t="s">
@@ -41251,20 +41257,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19.5" thickBot="1">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="96" t="s">
         <v>378</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="I1" s="112" t="s">
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="I1" s="114" t="s">
         <v>396</v>
       </c>
-      <c r="J1" s="112"/>
-      <c r="K1" s="112"/>
+      <c r="J1" s="114"/>
+      <c r="K1" s="114"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="81" t="s">
@@ -41533,10 +41539,10 @@
         <f t="shared" si="1"/>
         <v>0.93600000000000005</v>
       </c>
-      <c r="I10" s="94" t="s">
+      <c r="I10" s="96" t="s">
         <v>411</v>
       </c>
-      <c r="J10" s="94"/>
+      <c r="J10" s="96"/>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="5"/>
@@ -41571,18 +41577,18 @@
       <c r="G12" s="10"/>
     </row>
     <row r="14" spans="1:11" ht="19.5" thickBot="1">
-      <c r="A14" s="94" t="s">
+      <c r="A14" s="96" t="s">
         <v>401</v>
       </c>
-      <c r="B14" s="94"/>
-      <c r="C14" s="94"/>
-      <c r="D14" s="94"/>
-      <c r="E14" s="94"/>
-      <c r="F14" s="94"/>
-      <c r="G14" s="94"/>
-      <c r="H14" s="94"/>
-      <c r="I14" s="94"/>
-      <c r="J14" s="94"/>
+      <c r="B14" s="96"/>
+      <c r="C14" s="96"/>
+      <c r="D14" s="96"/>
+      <c r="E14" s="96"/>
+      <c r="F14" s="96"/>
+      <c r="G14" s="96"/>
+      <c r="H14" s="96"/>
+      <c r="I14" s="96"/>
+      <c r="J14" s="96"/>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="81" t="s">
@@ -41987,12 +41993,12 @@
     </row>
     <row r="27" spans="1:10" ht="19.5" thickBot="1"/>
     <row r="28" spans="1:10">
-      <c r="A28" s="102" t="s">
+      <c r="A28" s="104" t="s">
         <v>408</v>
       </c>
-      <c r="B28" s="103"/>
-      <c r="C28" s="103"/>
-      <c r="D28" s="103"/>
+      <c r="B28" s="105"/>
+      <c r="C28" s="105"/>
+      <c r="D28" s="105"/>
       <c r="E28" s="69">
         <f>DMIN(発注先別支払額一覧表12,H15,I28:I29)</f>
         <v>426955</v>
@@ -42005,12 +42011,12 @@
       </c>
     </row>
     <row r="29" spans="1:10" ht="19.5" thickBot="1">
-      <c r="A29" s="104" t="s">
+      <c r="A29" s="106" t="s">
         <v>409</v>
       </c>
-      <c r="B29" s="105"/>
-      <c r="C29" s="105"/>
-      <c r="D29" s="105"/>
+      <c r="B29" s="107"/>
+      <c r="C29" s="107"/>
+      <c r="D29" s="107"/>
       <c r="E29" s="14">
         <f>ROUND(DAVERAGE(発注先別支払額一覧表12,G15,J28:J29),0)</f>
         <v>21406</v>
@@ -42048,8 +42054,8 @@
   </sheetPr>
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:K1048576"/>
+    <sheetView showFormulas="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -42066,20 +42072,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19.5" thickBot="1">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="96" t="s">
         <v>378</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="I1" s="112" t="s">
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="I1" s="114" t="s">
         <v>396</v>
       </c>
-      <c r="J1" s="112"/>
-      <c r="K1" s="112"/>
+      <c r="J1" s="114"/>
+      <c r="K1" s="114"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="81" t="s">
@@ -42348,10 +42354,10 @@
         <f t="shared" si="1"/>
         <v>0.93600000000000005</v>
       </c>
-      <c r="I10" s="94" t="s">
+      <c r="I10" s="96" t="s">
         <v>411</v>
       </c>
-      <c r="J10" s="94"/>
+      <c r="J10" s="96"/>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="5"/>
@@ -42386,18 +42392,18 @@
       <c r="G12" s="10"/>
     </row>
     <row r="14" spans="1:11" ht="19.5" thickBot="1">
-      <c r="A14" s="94" t="s">
+      <c r="A14" s="96" t="s">
         <v>401</v>
       </c>
-      <c r="B14" s="94"/>
-      <c r="C14" s="94"/>
-      <c r="D14" s="94"/>
-      <c r="E14" s="94"/>
-      <c r="F14" s="94"/>
-      <c r="G14" s="94"/>
-      <c r="H14" s="94"/>
-      <c r="I14" s="94"/>
-      <c r="J14" s="94"/>
+      <c r="B14" s="96"/>
+      <c r="C14" s="96"/>
+      <c r="D14" s="96"/>
+      <c r="E14" s="96"/>
+      <c r="F14" s="96"/>
+      <c r="G14" s="96"/>
+      <c r="H14" s="96"/>
+      <c r="I14" s="96"/>
+      <c r="J14" s="96"/>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="81" t="s">
@@ -42802,12 +42808,12 @@
     </row>
     <row r="27" spans="1:10" ht="19.5" thickBot="1"/>
     <row r="28" spans="1:10">
-      <c r="A28" s="102" t="s">
+      <c r="A28" s="104" t="s">
         <v>408</v>
       </c>
-      <c r="B28" s="103"/>
-      <c r="C28" s="103"/>
-      <c r="D28" s="103"/>
+      <c r="B28" s="105"/>
+      <c r="C28" s="105"/>
+      <c r="D28" s="105"/>
       <c r="E28" s="69">
         <f>DMIN(発注先別支払額一覧表12,H15,I28:I29)</f>
         <v>426955</v>
@@ -42820,12 +42826,12 @@
       </c>
     </row>
     <row r="29" spans="1:10" ht="19.5" thickBot="1">
-      <c r="A29" s="104" t="s">
+      <c r="A29" s="106" t="s">
         <v>409</v>
       </c>
-      <c r="B29" s="105"/>
-      <c r="C29" s="105"/>
-      <c r="D29" s="105"/>
+      <c r="B29" s="107"/>
+      <c r="C29" s="107"/>
+      <c r="D29" s="107"/>
       <c r="E29" s="14">
         <f>ROUND(DAVERAGE(発注先別支払額一覧表12,G15,J28:J29),0)</f>
         <v>21406</v>
@@ -42861,7 +42867,7 @@
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -42880,21 +42886,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="19.5" thickBot="1">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="98" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="98"/>
       <c r="I1" s="19"/>
-      <c r="J1" s="96" t="s">
+      <c r="J1" s="98" t="s">
         <v>39</v>
       </c>
-      <c r="K1" s="96"/>
+      <c r="K1" s="98"/>
       <c r="L1" s="19"/>
     </row>
     <row r="2" spans="1:14">
@@ -43075,10 +43081,10 @@
         <v>3500</v>
       </c>
       <c r="I6" s="19"/>
-      <c r="J6" s="97" t="s">
+      <c r="J6" s="99" t="s">
         <v>57</v>
       </c>
-      <c r="K6" s="97"/>
+      <c r="K6" s="99"/>
       <c r="L6" s="19"/>
     </row>
     <row r="7" spans="1:14">
@@ -43165,19 +43171,19 @@
       <c r="L10" s="19"/>
     </row>
     <row r="11" spans="1:14" ht="19.5" thickBot="1">
-      <c r="A11" s="96" t="s">
+      <c r="A11" s="98" t="s">
         <v>61</v>
       </c>
-      <c r="B11" s="96"/>
-      <c r="C11" s="96"/>
-      <c r="D11" s="96"/>
-      <c r="E11" s="96"/>
-      <c r="F11" s="96"/>
-      <c r="G11" s="96"/>
-      <c r="H11" s="96"/>
-      <c r="I11" s="96"/>
-      <c r="J11" s="96"/>
-      <c r="K11" s="96"/>
+      <c r="B11" s="98"/>
+      <c r="C11" s="98"/>
+      <c r="D11" s="98"/>
+      <c r="E11" s="98"/>
+      <c r="F11" s="98"/>
+      <c r="G11" s="98"/>
+      <c r="H11" s="98"/>
+      <c r="I11" s="98"/>
+      <c r="J11" s="98"/>
+      <c r="K11" s="98"/>
       <c r="L11" s="19"/>
     </row>
     <row r="12" spans="1:14">
@@ -43834,11 +43840,11 @@
       <c r="N27" s="19"/>
     </row>
     <row r="28" spans="1:14" ht="19.5" thickBot="1">
-      <c r="A28" s="96" t="s">
+      <c r="A28" s="98" t="s">
         <v>68</v>
       </c>
-      <c r="B28" s="96"/>
-      <c r="C28" s="96"/>
+      <c r="B28" s="98"/>
+      <c r="C28" s="98"/>
       <c r="D28" s="19"/>
       <c r="E28" s="19"/>
       <c r="F28" s="19"/>
@@ -43993,7 +43999,7 @@
   </sheetPr>
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView showFormulas="1" workbookViewId="0">
+    <sheetView showFormulas="1" topLeftCell="A8" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -44015,21 +44021,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="19.5" thickBot="1">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="98" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="98"/>
       <c r="I1" s="19"/>
-      <c r="J1" s="96" t="s">
+      <c r="J1" s="98" t="s">
         <v>39</v>
       </c>
-      <c r="K1" s="96"/>
+      <c r="K1" s="98"/>
       <c r="L1" s="19"/>
     </row>
     <row r="2" spans="1:14">
@@ -44210,10 +44216,10 @@
         <v>3500</v>
       </c>
       <c r="I6" s="19"/>
-      <c r="J6" s="97" t="s">
+      <c r="J6" s="99" t="s">
         <v>57</v>
       </c>
-      <c r="K6" s="97"/>
+      <c r="K6" s="99"/>
       <c r="L6" s="19"/>
     </row>
     <row r="7" spans="1:14">
@@ -44300,19 +44306,19 @@
       <c r="L10" s="19"/>
     </row>
     <row r="11" spans="1:14" ht="19.5" thickBot="1">
-      <c r="A11" s="96" t="s">
+      <c r="A11" s="98" t="s">
         <v>61</v>
       </c>
-      <c r="B11" s="96"/>
-      <c r="C11" s="96"/>
-      <c r="D11" s="96"/>
-      <c r="E11" s="96"/>
-      <c r="F11" s="96"/>
-      <c r="G11" s="96"/>
-      <c r="H11" s="96"/>
-      <c r="I11" s="96"/>
-      <c r="J11" s="96"/>
-      <c r="K11" s="96"/>
+      <c r="B11" s="98"/>
+      <c r="C11" s="98"/>
+      <c r="D11" s="98"/>
+      <c r="E11" s="98"/>
+      <c r="F11" s="98"/>
+      <c r="G11" s="98"/>
+      <c r="H11" s="98"/>
+      <c r="I11" s="98"/>
+      <c r="J11" s="98"/>
+      <c r="K11" s="98"/>
       <c r="L11" s="19"/>
     </row>
     <row r="12" spans="1:14">
@@ -44969,11 +44975,11 @@
       <c r="N27" s="19"/>
     </row>
     <row r="28" spans="1:14" ht="19.5" thickBot="1">
-      <c r="A28" s="96" t="s">
+      <c r="A28" s="98" t="s">
         <v>68</v>
       </c>
-      <c r="B28" s="96"/>
-      <c r="C28" s="96"/>
+      <c r="B28" s="98"/>
+      <c r="C28" s="98"/>
       <c r="D28" s="19"/>
       <c r="E28" s="19"/>
       <c r="F28" s="19"/>
@@ -45128,8 +45134,8 @@
   </sheetPr>
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -45142,13 +45148,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="96" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="2" t="s">
@@ -45244,56 +45250,56 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A8" s="94" t="s">
+      <c r="A8" s="96" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="94"/>
-      <c r="C8" s="94"/>
-      <c r="D8" s="94"/>
-      <c r="E8" s="94"/>
-      <c r="F8" s="94"/>
-      <c r="G8" s="94"/>
-      <c r="H8" s="94"/>
-      <c r="I8" s="94"/>
-      <c r="J8" s="94"/>
-      <c r="K8" s="94"/>
-      <c r="L8" s="94"/>
+      <c r="B8" s="96"/>
+      <c r="C8" s="96"/>
+      <c r="D8" s="96"/>
+      <c r="E8" s="96"/>
+      <c r="F8" s="96"/>
+      <c r="G8" s="96"/>
+      <c r="H8" s="96"/>
+      <c r="I8" s="96"/>
+      <c r="J8" s="96"/>
+      <c r="K8" s="96"/>
+      <c r="L8" s="96"/>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="94" t="s">
         <v>81</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="95" t="s">
         <v>82</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="95" t="s">
         <v>72</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="95" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="95" t="s">
         <v>83</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="95" t="s">
         <v>74</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="95" t="s">
         <v>84</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" s="95" t="s">
         <v>85</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="I9" s="95" t="s">
         <v>86</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="J9" s="95" t="s">
         <v>87</v>
       </c>
-      <c r="K9" s="40" t="s">
+      <c r="K9" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="L9" s="41" t="s">
+      <c r="L9" s="22" t="s">
         <v>97</v>
       </c>
     </row>
@@ -45718,12 +45724,12 @@
     </row>
     <row r="21" spans="1:12" ht="19.5" thickBot="1"/>
     <row r="22" spans="1:12">
-      <c r="A22" s="100" t="s">
+      <c r="A22" s="102" t="s">
         <v>98</v>
       </c>
-      <c r="B22" s="101"/>
-      <c r="C22" s="101"/>
-      <c r="D22" s="101"/>
+      <c r="B22" s="103"/>
+      <c r="C22" s="103"/>
+      <c r="D22" s="103"/>
       <c r="E22" s="18">
         <f>DCOUNT(請求金額一覧表3,11,$G$22:$G$23)</f>
         <v>5</v>
@@ -45733,12 +45739,12 @@
       </c>
     </row>
     <row r="23" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A23" s="98" t="s">
+      <c r="A23" s="100" t="s">
         <v>99</v>
       </c>
-      <c r="B23" s="99"/>
-      <c r="C23" s="99"/>
-      <c r="D23" s="99"/>
+      <c r="B23" s="101"/>
+      <c r="C23" s="101"/>
+      <c r="D23" s="101"/>
       <c r="E23" s="14">
         <f>DSUM(請求金額一覧表3,9,G24:G25)</f>
         <v>525610</v>
@@ -45782,7 +45788,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView showFormulas="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:L1048576"/>
+      <selection activeCell="A22" sqref="A22:D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -45802,13 +45808,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="96" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="2" t="s">
@@ -45904,20 +45910,20 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A8" s="94" t="s">
+      <c r="A8" s="96" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="94"/>
-      <c r="C8" s="94"/>
-      <c r="D8" s="94"/>
-      <c r="E8" s="94"/>
-      <c r="F8" s="94"/>
-      <c r="G8" s="94"/>
-      <c r="H8" s="94"/>
-      <c r="I8" s="94"/>
-      <c r="J8" s="94"/>
-      <c r="K8" s="94"/>
-      <c r="L8" s="94"/>
+      <c r="B8" s="96"/>
+      <c r="C8" s="96"/>
+      <c r="D8" s="96"/>
+      <c r="E8" s="96"/>
+      <c r="F8" s="96"/>
+      <c r="G8" s="96"/>
+      <c r="H8" s="96"/>
+      <c r="I8" s="96"/>
+      <c r="J8" s="96"/>
+      <c r="K8" s="96"/>
+      <c r="L8" s="96"/>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="2" t="s">
@@ -46378,12 +46384,12 @@
     </row>
     <row r="21" spans="1:12" ht="19.5" thickBot="1"/>
     <row r="22" spans="1:12">
-      <c r="A22" s="100" t="s">
+      <c r="A22" s="102" t="s">
         <v>98</v>
       </c>
-      <c r="B22" s="101"/>
-      <c r="C22" s="101"/>
-      <c r="D22" s="101"/>
+      <c r="B22" s="103"/>
+      <c r="C22" s="103"/>
+      <c r="D22" s="103"/>
       <c r="E22" s="18">
         <f>DCOUNT(請求金額一覧表3,11,$G$22:$G$23)</f>
         <v>5</v>
@@ -46393,12 +46399,12 @@
       </c>
     </row>
     <row r="23" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A23" s="98" t="s">
+      <c r="A23" s="100" t="s">
         <v>99</v>
       </c>
-      <c r="B23" s="99"/>
-      <c r="C23" s="99"/>
-      <c r="D23" s="99"/>
+      <c r="B23" s="101"/>
+      <c r="C23" s="101"/>
+      <c r="D23" s="101"/>
       <c r="E23" s="14">
         <f>DSUM(請求金額一覧表3,9,G24:G25)</f>
         <v>525610</v>
@@ -46457,14 +46463,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="108" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
+      <c r="B1" s="108"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
     </row>
     <row r="2" spans="1:12" ht="19.5" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -46485,14 +46491,14 @@
       <c r="F2" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="H2" s="94" t="s">
+      <c r="H2" s="96" t="s">
         <v>134</v>
       </c>
-      <c r="I2" s="94"/>
-      <c r="K2" s="95" t="s">
+      <c r="I2" s="96"/>
+      <c r="K2" s="97" t="s">
         <v>135</v>
       </c>
-      <c r="L2" s="95"/>
+      <c r="L2" s="97"/>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="5">
@@ -46631,20 +46637,20 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A8" s="94" t="s">
+      <c r="A8" s="96" t="s">
         <v>115</v>
       </c>
-      <c r="B8" s="94"/>
-      <c r="C8" s="94"/>
-      <c r="D8" s="94"/>
-      <c r="E8" s="94"/>
-      <c r="F8" s="94"/>
-      <c r="G8" s="94"/>
-      <c r="H8" s="94"/>
-      <c r="I8" s="94"/>
-      <c r="J8" s="94"/>
-      <c r="K8" s="94"/>
-      <c r="L8" s="94"/>
+      <c r="B8" s="96"/>
+      <c r="C8" s="96"/>
+      <c r="D8" s="96"/>
+      <c r="E8" s="96"/>
+      <c r="F8" s="96"/>
+      <c r="G8" s="96"/>
+      <c r="H8" s="96"/>
+      <c r="I8" s="96"/>
+      <c r="J8" s="96"/>
+      <c r="K8" s="96"/>
+      <c r="L8" s="96"/>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="2" t="s">
@@ -47094,12 +47100,12 @@
     </row>
     <row r="21" spans="1:12" ht="19.5" thickBot="1"/>
     <row r="22" spans="1:12">
-      <c r="B22" s="102" t="s">
+      <c r="B22" s="104" t="s">
         <v>143</v>
       </c>
-      <c r="C22" s="103"/>
-      <c r="D22" s="103"/>
-      <c r="E22" s="103"/>
+      <c r="C22" s="105"/>
+      <c r="D22" s="105"/>
+      <c r="E22" s="105"/>
       <c r="F22" s="69">
         <f>DSUM(依頼先別加工賃一覧表4,G9,$I$22:$I$23)</f>
         <v>1921898</v>
@@ -47112,12 +47118,12 @@
       </c>
     </row>
     <row r="23" spans="1:12" ht="19.5" thickBot="1">
-      <c r="B23" s="104" t="s">
+      <c r="B23" s="106" t="s">
         <v>142</v>
       </c>
-      <c r="C23" s="105"/>
-      <c r="D23" s="105"/>
-      <c r="E23" s="105"/>
+      <c r="C23" s="107"/>
+      <c r="D23" s="107"/>
+      <c r="E23" s="107"/>
       <c r="F23" s="14">
         <f>ROUND(DAVERAGE(依頼先別加工賃一覧表4,J9,$K$22:$K$23),0)</f>
         <v>455239</v>
@@ -47156,7 +47162,7 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView showFormulas="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:L1048576"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -47176,14 +47182,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="108" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
+      <c r="B1" s="108"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
     </row>
     <row r="2" spans="1:12" ht="19.5" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -47204,14 +47210,14 @@
       <c r="F2" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="H2" s="94" t="s">
+      <c r="H2" s="96" t="s">
         <v>134</v>
       </c>
-      <c r="I2" s="94"/>
-      <c r="K2" s="95" t="s">
+      <c r="I2" s="96"/>
+      <c r="K2" s="97" t="s">
         <v>135</v>
       </c>
-      <c r="L2" s="95"/>
+      <c r="L2" s="97"/>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="5">
@@ -47350,20 +47356,20 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A8" s="94" t="s">
+      <c r="A8" s="96" t="s">
         <v>115</v>
       </c>
-      <c r="B8" s="94"/>
-      <c r="C8" s="94"/>
-      <c r="D8" s="94"/>
-      <c r="E8" s="94"/>
-      <c r="F8" s="94"/>
-      <c r="G8" s="94"/>
-      <c r="H8" s="94"/>
-      <c r="I8" s="94"/>
-      <c r="J8" s="94"/>
-      <c r="K8" s="94"/>
-      <c r="L8" s="94"/>
+      <c r="B8" s="96"/>
+      <c r="C8" s="96"/>
+      <c r="D8" s="96"/>
+      <c r="E8" s="96"/>
+      <c r="F8" s="96"/>
+      <c r="G8" s="96"/>
+      <c r="H8" s="96"/>
+      <c r="I8" s="96"/>
+      <c r="J8" s="96"/>
+      <c r="K8" s="96"/>
+      <c r="L8" s="96"/>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="2" t="s">
@@ -47813,12 +47819,12 @@
     </row>
     <row r="21" spans="1:12" ht="19.5" thickBot="1"/>
     <row r="22" spans="1:12">
-      <c r="B22" s="102" t="s">
+      <c r="B22" s="104" t="s">
         <v>143</v>
       </c>
-      <c r="C22" s="103"/>
-      <c r="D22" s="103"/>
-      <c r="E22" s="103"/>
+      <c r="C22" s="105"/>
+      <c r="D22" s="105"/>
+      <c r="E22" s="105"/>
       <c r="F22" s="69">
         <f>DSUM(依頼先別加工賃一覧表4,G9,$I$22:$I$23)</f>
         <v>1921898</v>
@@ -47831,12 +47837,12 @@
       </c>
     </row>
     <row r="23" spans="1:12" ht="19.5" thickBot="1">
-      <c r="B23" s="104" t="s">
+      <c r="B23" s="106" t="s">
         <v>142</v>
       </c>
-      <c r="C23" s="105"/>
-      <c r="D23" s="105"/>
-      <c r="E23" s="105"/>
+      <c r="C23" s="107"/>
+      <c r="D23" s="107"/>
+      <c r="E23" s="107"/>
       <c r="F23" s="14">
         <f>ROUND(DAVERAGE(依頼先別加工賃一覧表4,J9,$K$22:$K$23),0)</f>
         <v>455239</v>
@@ -47887,22 +47893,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="96" t="s">
         <v>148</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="H1" s="95" t="s">
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="H1" s="97" t="s">
         <v>159</v>
       </c>
-      <c r="I1" s="95"/>
-      <c r="K1" s="95" t="s">
+      <c r="I1" s="97"/>
+      <c r="K1" s="97" t="s">
         <v>163</v>
       </c>
-      <c r="L1" s="95"/>
+      <c r="L1" s="97"/>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="2" t="s">
@@ -48067,20 +48073,20 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A8" s="94" t="s">
+      <c r="A8" s="96" t="s">
         <v>174</v>
       </c>
-      <c r="B8" s="94"/>
-      <c r="C8" s="94"/>
-      <c r="D8" s="94"/>
-      <c r="E8" s="94"/>
-      <c r="F8" s="94"/>
-      <c r="G8" s="94"/>
-      <c r="H8" s="94"/>
-      <c r="I8" s="94"/>
-      <c r="J8" s="94"/>
-      <c r="K8" s="94"/>
-      <c r="L8" s="94"/>
+      <c r="B8" s="96"/>
+      <c r="C8" s="96"/>
+      <c r="D8" s="96"/>
+      <c r="E8" s="96"/>
+      <c r="F8" s="96"/>
+      <c r="G8" s="96"/>
+      <c r="H8" s="96"/>
+      <c r="I8" s="96"/>
+      <c r="J8" s="96"/>
+      <c r="K8" s="96"/>
+      <c r="L8" s="96"/>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="2" t="s">
@@ -48755,11 +48761,11 @@
       <c r="L24" s="10"/>
     </row>
     <row r="26" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A26" s="107" t="s">
+      <c r="A26" s="109" t="s">
         <v>181</v>
       </c>
-      <c r="B26" s="107"/>
-      <c r="C26" s="107"/>
+      <c r="B26" s="109"/>
+      <c r="C26" s="109"/>
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="2" t="s">

</xml_diff>

<commit_message>
R5 12 21 office
</commit_message>
<xml_diff>
--- a/inside_office/excel/準1級.xlsx
+++ b/inside_office/excel/準1級.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20404"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A39EA00-FF06-4D65-A26E-64078C84D79C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C11365-4112-490A-8309-B7D5F7EA97BF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10635" windowHeight="11445" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285" tabRatio="976" firstSheet="4" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="準1-1" sheetId="1" r:id="rId1"/>
@@ -3371,12 +3371,18 @@
       <charset val="128"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="16">
@@ -3606,7 +3612,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3781,11 +3787,14 @@
     <xf numFmtId="40" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="40" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -28127,16 +28136,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19.5" thickBot="1">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="97" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
     </row>
     <row r="2" spans="1:11" ht="19.5" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -28163,10 +28172,10 @@
       <c r="H2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="97" t="s">
+      <c r="J2" s="98" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="97"/>
+      <c r="K2" s="98"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="5">
@@ -28349,19 +28358,19 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="19.5" thickBot="1">
-      <c r="A10" s="96" t="s">
+      <c r="A10" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="96"/>
-      <c r="C10" s="96"/>
-      <c r="D10" s="96"/>
-      <c r="E10" s="96"/>
-      <c r="F10" s="96"/>
-      <c r="G10" s="96"/>
-      <c r="H10" s="96"/>
-      <c r="I10" s="96"/>
-      <c r="J10" s="96"/>
-      <c r="K10" s="96"/>
+      <c r="B10" s="97"/>
+      <c r="C10" s="97"/>
+      <c r="D10" s="97"/>
+      <c r="E10" s="97"/>
+      <c r="F10" s="97"/>
+      <c r="G10" s="97"/>
+      <c r="H10" s="97"/>
+      <c r="I10" s="97"/>
+      <c r="J10" s="97"/>
+      <c r="K10" s="97"/>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="2" t="s">
@@ -28943,11 +28952,11 @@
       <c r="K25" s="10"/>
     </row>
     <row r="27" spans="1:11" ht="19.5" thickBot="1">
-      <c r="A27" s="97" t="s">
+      <c r="A27" s="98" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="97"/>
-      <c r="C27" s="97"/>
+      <c r="B27" s="98"/>
+      <c r="C27" s="98"/>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="2" t="s">
@@ -29059,22 +29068,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="97" t="s">
         <v>148</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="H1" s="97" t="s">
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="H1" s="98" t="s">
         <v>159</v>
       </c>
-      <c r="I1" s="97"/>
-      <c r="K1" s="97" t="s">
+      <c r="I1" s="98"/>
+      <c r="K1" s="98" t="s">
         <v>163</v>
       </c>
-      <c r="L1" s="97"/>
+      <c r="L1" s="98"/>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="2" t="s">
@@ -29239,20 +29248,20 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A8" s="96" t="s">
+      <c r="A8" s="97" t="s">
         <v>174</v>
       </c>
-      <c r="B8" s="96"/>
-      <c r="C8" s="96"/>
-      <c r="D8" s="96"/>
-      <c r="E8" s="96"/>
-      <c r="F8" s="96"/>
-      <c r="G8" s="96"/>
-      <c r="H8" s="96"/>
-      <c r="I8" s="96"/>
-      <c r="J8" s="96"/>
-      <c r="K8" s="96"/>
-      <c r="L8" s="96"/>
+      <c r="B8" s="97"/>
+      <c r="C8" s="97"/>
+      <c r="D8" s="97"/>
+      <c r="E8" s="97"/>
+      <c r="F8" s="97"/>
+      <c r="G8" s="97"/>
+      <c r="H8" s="97"/>
+      <c r="I8" s="97"/>
+      <c r="J8" s="97"/>
+      <c r="K8" s="97"/>
+      <c r="L8" s="97"/>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="2" t="s">
@@ -29927,11 +29936,11 @@
       <c r="L24" s="10"/>
     </row>
     <row r="26" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A26" s="109" t="s">
+      <c r="A26" s="110" t="s">
         <v>181</v>
       </c>
-      <c r="B26" s="109"/>
-      <c r="C26" s="109"/>
+      <c r="B26" s="110"/>
+      <c r="C26" s="110"/>
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="55" t="s">
@@ -30060,16 +30069,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="19.5" thickBot="1">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="97" t="s">
         <v>183</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
     </row>
     <row r="2" spans="1:14" ht="19.5" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -30096,14 +30105,14 @@
       <c r="H2" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="J2" s="97" t="s">
+      <c r="J2" s="98" t="s">
         <v>202</v>
       </c>
-      <c r="K2" s="97"/>
-      <c r="M2" s="96" t="s">
+      <c r="K2" s="98"/>
+      <c r="M2" s="97" t="s">
         <v>158</v>
       </c>
-      <c r="N2" s="96"/>
+      <c r="N2" s="97"/>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="5">
@@ -30360,10 +30369,10 @@
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
-      <c r="M9" s="96" t="s">
+      <c r="M9" s="97" t="s">
         <v>224</v>
       </c>
-      <c r="N9" s="96"/>
+      <c r="N9" s="97"/>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="5">
@@ -30426,10 +30435,10 @@
         <f t="shared" si="1"/>
         <v>63</v>
       </c>
-      <c r="J11" s="97" t="s">
+      <c r="J11" s="98" t="s">
         <v>208</v>
       </c>
-      <c r="K11" s="97"/>
+      <c r="K11" s="98"/>
       <c r="M11" s="5">
         <v>1</v>
       </c>
@@ -30496,20 +30505,20 @@
       </c>
     </row>
     <row r="15" spans="1:14" ht="19.5" thickBot="1">
-      <c r="A15" s="108" t="s">
+      <c r="A15" s="109" t="s">
         <v>211</v>
       </c>
-      <c r="B15" s="108"/>
-      <c r="C15" s="108"/>
-      <c r="D15" s="108"/>
-      <c r="E15" s="108"/>
-      <c r="F15" s="108"/>
-      <c r="G15" s="108"/>
-      <c r="H15" s="108"/>
-      <c r="I15" s="108"/>
-      <c r="J15" s="108"/>
-      <c r="K15" s="108"/>
-      <c r="L15" s="108"/>
+      <c r="B15" s="109"/>
+      <c r="C15" s="109"/>
+      <c r="D15" s="109"/>
+      <c r="E15" s="109"/>
+      <c r="F15" s="109"/>
+      <c r="G15" s="109"/>
+      <c r="H15" s="109"/>
+      <c r="I15" s="109"/>
+      <c r="J15" s="109"/>
+      <c r="K15" s="109"/>
+      <c r="L15" s="109"/>
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="2" t="s">
@@ -31019,12 +31028,12 @@
     </row>
     <row r="29" spans="1:12" ht="19.5" thickBot="1"/>
     <row r="30" spans="1:12">
-      <c r="A30" s="104" t="s">
+      <c r="A30" s="105" t="s">
         <v>225</v>
       </c>
-      <c r="B30" s="105"/>
-      <c r="C30" s="105"/>
-      <c r="D30" s="105"/>
+      <c r="B30" s="106"/>
+      <c r="C30" s="106"/>
+      <c r="D30" s="106"/>
       <c r="E30" s="69">
         <f>ROUND(DAVERAGE(総支給額一覧表6,K16,$I$30:$I$31),0)</f>
         <v>327735</v>
@@ -31037,12 +31046,12 @@
       </c>
     </row>
     <row r="31" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A31" s="106" t="s">
+      <c r="A31" s="107" t="s">
         <v>226</v>
       </c>
-      <c r="B31" s="107"/>
-      <c r="C31" s="107"/>
-      <c r="D31" s="107"/>
+      <c r="B31" s="108"/>
+      <c r="C31" s="108"/>
+      <c r="D31" s="108"/>
       <c r="E31" s="14">
         <f>DSUM(総支給額一覧表6,G16,$K$30:$K$31)</f>
         <v>68815</v>
@@ -31105,16 +31114,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="19.5" thickBot="1">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="97" t="s">
         <v>183</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
     </row>
     <row r="2" spans="1:14" ht="19.5" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -31141,14 +31150,14 @@
       <c r="H2" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="J2" s="97" t="s">
+      <c r="J2" s="98" t="s">
         <v>202</v>
       </c>
-      <c r="K2" s="97"/>
-      <c r="M2" s="96" t="s">
+      <c r="K2" s="98"/>
+      <c r="M2" s="97" t="s">
         <v>134</v>
       </c>
-      <c r="N2" s="96"/>
+      <c r="N2" s="97"/>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="5">
@@ -31405,10 +31414,10 @@
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
-      <c r="M9" s="96" t="s">
+      <c r="M9" s="97" t="s">
         <v>224</v>
       </c>
-      <c r="N9" s="96"/>
+      <c r="N9" s="97"/>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="5">
@@ -31471,10 +31480,10 @@
         <f t="shared" si="1"/>
         <v>63</v>
       </c>
-      <c r="J11" s="97" t="s">
+      <c r="J11" s="98" t="s">
         <v>208</v>
       </c>
-      <c r="K11" s="97"/>
+      <c r="K11" s="98"/>
       <c r="M11" s="5">
         <v>1</v>
       </c>
@@ -31541,20 +31550,20 @@
       </c>
     </row>
     <row r="15" spans="1:14" ht="19.5" thickBot="1">
-      <c r="A15" s="108" t="s">
+      <c r="A15" s="109" t="s">
         <v>211</v>
       </c>
-      <c r="B15" s="108"/>
-      <c r="C15" s="108"/>
-      <c r="D15" s="108"/>
-      <c r="E15" s="108"/>
-      <c r="F15" s="108"/>
-      <c r="G15" s="108"/>
-      <c r="H15" s="108"/>
-      <c r="I15" s="108"/>
-      <c r="J15" s="108"/>
-      <c r="K15" s="108"/>
-      <c r="L15" s="108"/>
+      <c r="B15" s="109"/>
+      <c r="C15" s="109"/>
+      <c r="D15" s="109"/>
+      <c r="E15" s="109"/>
+      <c r="F15" s="109"/>
+      <c r="G15" s="109"/>
+      <c r="H15" s="109"/>
+      <c r="I15" s="109"/>
+      <c r="J15" s="109"/>
+      <c r="K15" s="109"/>
+      <c r="L15" s="109"/>
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="2" t="s">
@@ -32064,12 +32073,12 @@
     </row>
     <row r="29" spans="1:12" ht="19.5" thickBot="1"/>
     <row r="30" spans="1:12">
-      <c r="A30" s="104" t="s">
+      <c r="A30" s="105" t="s">
         <v>225</v>
       </c>
-      <c r="B30" s="105"/>
-      <c r="C30" s="105"/>
-      <c r="D30" s="105"/>
+      <c r="B30" s="106"/>
+      <c r="C30" s="106"/>
+      <c r="D30" s="106"/>
       <c r="E30" s="69">
         <f>ROUND(DAVERAGE(総支給額一覧表6,K16,$I$30:$I$31),0)</f>
         <v>327735</v>
@@ -32082,12 +32091,12 @@
       </c>
     </row>
     <row r="31" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A31" s="106" t="s">
+      <c r="A31" s="107" t="s">
         <v>226</v>
       </c>
-      <c r="B31" s="107"/>
-      <c r="C31" s="107"/>
-      <c r="D31" s="107"/>
+      <c r="B31" s="108"/>
+      <c r="C31" s="108"/>
+      <c r="D31" s="108"/>
       <c r="E31" s="14">
         <f>DSUM(総支給額一覧表6,G16,$K$30:$K$31)</f>
         <v>68815</v>
@@ -32138,16 +32147,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" thickBot="1">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="97" t="s">
         <v>229</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
@@ -32333,17 +32342,17 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="19.5" thickBot="1">
-      <c r="A10" s="96" t="s">
+      <c r="A10" s="97" t="s">
         <v>246</v>
       </c>
-      <c r="B10" s="96"/>
-      <c r="C10" s="96"/>
-      <c r="D10" s="96"/>
-      <c r="E10" s="96"/>
-      <c r="F10" s="96"/>
-      <c r="G10" s="96"/>
-      <c r="H10" s="96"/>
-      <c r="I10" s="96"/>
+      <c r="B10" s="97"/>
+      <c r="C10" s="97"/>
+      <c r="D10" s="97"/>
+      <c r="E10" s="97"/>
+      <c r="F10" s="97"/>
+      <c r="G10" s="97"/>
+      <c r="H10" s="97"/>
+      <c r="I10" s="97"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="2" t="s">
@@ -32694,18 +32703,18 @@
       <c r="I21" s="10"/>
     </row>
     <row r="23" spans="1:9" ht="19.5" thickBot="1">
-      <c r="A23" s="96" t="s">
+      <c r="A23" s="97" t="s">
         <v>247</v>
       </c>
-      <c r="B23" s="96"/>
-      <c r="C23" s="96"/>
-      <c r="D23" s="96"/>
+      <c r="B23" s="97"/>
+      <c r="C23" s="97"/>
+      <c r="D23" s="97"/>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="112" t="s">
+      <c r="A24" s="113" t="s">
         <v>231</v>
       </c>
-      <c r="B24" s="113"/>
+      <c r="B24" s="114"/>
       <c r="C24" s="3" t="s">
         <v>244</v>
       </c>
@@ -32726,10 +32735,10 @@
       </c>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="110" t="s">
+      <c r="A25" s="111" t="s">
         <v>239</v>
       </c>
-      <c r="B25" s="111"/>
+      <c r="B25" s="112"/>
       <c r="C25" s="11">
         <f>DSUM(株式売却一覧表7,C$24,$F$24:$F$25)</f>
         <v>15429</v>
@@ -32752,10 +32761,10 @@
       </c>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26" s="110" t="s">
+      <c r="A26" s="111" t="s">
         <v>240</v>
       </c>
-      <c r="B26" s="111"/>
+      <c r="B26" s="112"/>
       <c r="C26" s="11">
         <f>DSUM(株式売却一覧表7,C$24,$G$24:$G$25)</f>
         <v>24961</v>
@@ -32766,10 +32775,10 @@
       </c>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="110" t="s">
+      <c r="A27" s="111" t="s">
         <v>241</v>
       </c>
-      <c r="B27" s="111"/>
+      <c r="B27" s="112"/>
       <c r="C27" s="11">
         <f>DSUM(株式売却一覧表7,C$24,$H$24:$H$25)</f>
         <v>19858</v>
@@ -32780,10 +32789,10 @@
       </c>
     </row>
     <row r="28" spans="1:9" ht="19.5" thickBot="1">
-      <c r="A28" s="106" t="s">
+      <c r="A28" s="107" t="s">
         <v>243</v>
       </c>
-      <c r="B28" s="107"/>
+      <c r="B28" s="108"/>
       <c r="C28" s="13">
         <f>DSUM(株式売却一覧表7,C$24,$I$24:$I$25)</f>
         <v>22820</v>
@@ -32839,16 +32848,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" thickBot="1">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="97" t="s">
         <v>229</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
@@ -33034,17 +33043,17 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="19.5" thickBot="1">
-      <c r="A10" s="96" t="s">
+      <c r="A10" s="97" t="s">
         <v>246</v>
       </c>
-      <c r="B10" s="96"/>
-      <c r="C10" s="96"/>
-      <c r="D10" s="96"/>
-      <c r="E10" s="96"/>
-      <c r="F10" s="96"/>
-      <c r="G10" s="96"/>
-      <c r="H10" s="96"/>
-      <c r="I10" s="96"/>
+      <c r="B10" s="97"/>
+      <c r="C10" s="97"/>
+      <c r="D10" s="97"/>
+      <c r="E10" s="97"/>
+      <c r="F10" s="97"/>
+      <c r="G10" s="97"/>
+      <c r="H10" s="97"/>
+      <c r="I10" s="97"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="2" t="s">
@@ -33395,18 +33404,18 @@
       <c r="I21" s="10"/>
     </row>
     <row r="23" spans="1:9" ht="19.5" thickBot="1">
-      <c r="A23" s="96" t="s">
+      <c r="A23" s="97" t="s">
         <v>247</v>
       </c>
-      <c r="B23" s="96"/>
-      <c r="C23" s="96"/>
-      <c r="D23" s="96"/>
+      <c r="B23" s="97"/>
+      <c r="C23" s="97"/>
+      <c r="D23" s="97"/>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="112" t="s">
+      <c r="A24" s="113" t="s">
         <v>231</v>
       </c>
-      <c r="B24" s="113"/>
+      <c r="B24" s="114"/>
       <c r="C24" s="3" t="s">
         <v>244</v>
       </c>
@@ -33427,10 +33436,10 @@
       </c>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="110" t="s">
+      <c r="A25" s="111" t="s">
         <v>239</v>
       </c>
-      <c r="B25" s="111"/>
+      <c r="B25" s="112"/>
       <c r="C25" s="11">
         <f>DSUM(株式売却一覧表7,C$24,$F$24:$F$25)</f>
         <v>15429</v>
@@ -33453,10 +33462,10 @@
       </c>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26" s="110" t="s">
+      <c r="A26" s="111" t="s">
         <v>240</v>
       </c>
-      <c r="B26" s="111"/>
+      <c r="B26" s="112"/>
       <c r="C26" s="11">
         <f>DSUM(株式売却一覧表7,C$24,$G$24:$G$25)</f>
         <v>24961</v>
@@ -33467,10 +33476,10 @@
       </c>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="110" t="s">
+      <c r="A27" s="111" t="s">
         <v>241</v>
       </c>
-      <c r="B27" s="111"/>
+      <c r="B27" s="112"/>
       <c r="C27" s="11">
         <f>DSUM(株式売却一覧表7,C$24,$H$24:$H$25)</f>
         <v>19858</v>
@@ -33481,10 +33490,10 @@
       </c>
     </row>
     <row r="28" spans="1:9" ht="19.5" thickBot="1">
-      <c r="A28" s="106" t="s">
+      <c r="A28" s="107" t="s">
         <v>243</v>
       </c>
-      <c r="B28" s="107"/>
+      <c r="B28" s="108"/>
       <c r="C28" s="13">
         <f>DSUM(株式売却一覧表7,C$24,$I$24:$I$25)</f>
         <v>22820</v>
@@ -33539,22 +33548,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19.5" thickBot="1">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="97" t="s">
         <v>250</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="K1" s="96" t="s">
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
+      <c r="K1" s="97" t="s">
         <v>262</v>
       </c>
-      <c r="L1" s="96"/>
-      <c r="M1" s="96"/>
+      <c r="L1" s="97"/>
+      <c r="M1" s="97"/>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="2" t="s">
@@ -33937,22 +33946,22 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="19.5" thickBot="1">
-      <c r="A14" s="96" t="s">
+      <c r="A14" s="97" t="s">
         <v>267</v>
       </c>
-      <c r="B14" s="96"/>
-      <c r="C14" s="96"/>
-      <c r="D14" s="96"/>
-      <c r="E14" s="96"/>
-      <c r="F14" s="96"/>
-      <c r="G14" s="96"/>
-      <c r="H14" s="96"/>
-      <c r="I14" s="96"/>
-      <c r="J14" s="96"/>
-      <c r="L14" s="96" t="s">
+      <c r="B14" s="97"/>
+      <c r="C14" s="97"/>
+      <c r="D14" s="97"/>
+      <c r="E14" s="97"/>
+      <c r="F14" s="97"/>
+      <c r="G14" s="97"/>
+      <c r="H14" s="97"/>
+      <c r="I14" s="97"/>
+      <c r="J14" s="97"/>
+      <c r="L14" s="97" t="s">
         <v>271</v>
       </c>
-      <c r="M14" s="96"/>
+      <c r="M14" s="97"/>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="2" t="s">
@@ -34416,12 +34425,12 @@
     </row>
     <row r="28" spans="1:13" ht="19.5" thickBot="1"/>
     <row r="29" spans="1:13">
-      <c r="A29" s="104" t="s">
+      <c r="A29" s="105" t="s">
         <v>272</v>
       </c>
-      <c r="B29" s="105"/>
-      <c r="C29" s="105"/>
-      <c r="D29" s="105"/>
+      <c r="B29" s="106"/>
+      <c r="C29" s="106"/>
+      <c r="D29" s="106"/>
       <c r="E29" s="18">
         <f>DCOUNT(請求額一覧表8, E15, G29:G30)</f>
         <v>3</v>
@@ -34434,12 +34443,12 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="19.5" thickBot="1">
-      <c r="A30" s="106" t="s">
+      <c r="A30" s="107" t="s">
         <v>273</v>
       </c>
-      <c r="B30" s="107"/>
-      <c r="C30" s="107"/>
-      <c r="D30" s="107"/>
+      <c r="B30" s="108"/>
+      <c r="C30" s="108"/>
+      <c r="D30" s="108"/>
       <c r="E30" s="14">
         <f>ROUND(DAVERAGE(請求額一覧表8,H15, I29:I30),0)</f>
         <v>509766</v>
@@ -34478,7 +34487,7 @@
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView showFormulas="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="A2" sqref="A1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -34498,22 +34507,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19.5" thickBot="1">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="97" t="s">
         <v>250</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="K1" s="96" t="s">
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
+      <c r="K1" s="97" t="s">
         <v>262</v>
       </c>
-      <c r="L1" s="96"/>
-      <c r="M1" s="96"/>
+      <c r="L1" s="97"/>
+      <c r="M1" s="97"/>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="2" t="s">
@@ -34896,22 +34905,22 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="19.5" thickBot="1">
-      <c r="A14" s="96" t="s">
+      <c r="A14" s="97" t="s">
         <v>267</v>
       </c>
-      <c r="B14" s="96"/>
-      <c r="C14" s="96"/>
-      <c r="D14" s="96"/>
-      <c r="E14" s="96"/>
-      <c r="F14" s="96"/>
-      <c r="G14" s="96"/>
-      <c r="H14" s="96"/>
-      <c r="I14" s="96"/>
-      <c r="J14" s="96"/>
-      <c r="L14" s="96" t="s">
+      <c r="B14" s="97"/>
+      <c r="C14" s="97"/>
+      <c r="D14" s="97"/>
+      <c r="E14" s="97"/>
+      <c r="F14" s="97"/>
+      <c r="G14" s="97"/>
+      <c r="H14" s="97"/>
+      <c r="I14" s="97"/>
+      <c r="J14" s="97"/>
+      <c r="L14" s="97" t="s">
         <v>271</v>
       </c>
-      <c r="M14" s="96"/>
+      <c r="M14" s="97"/>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="2" t="s">
@@ -35375,12 +35384,12 @@
     </row>
     <row r="28" spans="1:13" ht="19.5" thickBot="1"/>
     <row r="29" spans="1:13">
-      <c r="A29" s="104" t="s">
+      <c r="A29" s="105" t="s">
         <v>272</v>
       </c>
-      <c r="B29" s="105"/>
-      <c r="C29" s="105"/>
-      <c r="D29" s="105"/>
+      <c r="B29" s="106"/>
+      <c r="C29" s="106"/>
+      <c r="D29" s="106"/>
       <c r="E29" s="18">
         <f>DCOUNT(請求額一覧表8, E15, G29:G30)</f>
         <v>3</v>
@@ -35393,12 +35402,12 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="19.5" thickBot="1">
-      <c r="A30" s="106" t="s">
+      <c r="A30" s="107" t="s">
         <v>273</v>
       </c>
-      <c r="B30" s="107"/>
-      <c r="C30" s="107"/>
-      <c r="D30" s="107"/>
+      <c r="B30" s="108"/>
+      <c r="C30" s="108"/>
+      <c r="D30" s="108"/>
       <c r="E30" s="14">
         <f>ROUND(DAVERAGE(請求額一覧表8,H15, I29:I30),0)</f>
         <v>509766</v>
@@ -35449,22 +35458,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19.5" thickBot="1">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="97" t="s">
         <v>278</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="J1" s="96" t="s">
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="J1" s="97" t="s">
         <v>300</v>
       </c>
-      <c r="K1" s="96"/>
-      <c r="L1" s="96"/>
-      <c r="M1" s="96"/>
+      <c r="K1" s="97"/>
+      <c r="L1" s="97"/>
+      <c r="M1" s="97"/>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="2" t="s">
@@ -35824,21 +35833,21 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="19.5" thickBot="1">
-      <c r="A14" s="96" t="s">
+      <c r="A14" s="97" t="s">
         <v>283</v>
       </c>
-      <c r="B14" s="96"/>
-      <c r="C14" s="96"/>
-      <c r="D14" s="96"/>
-      <c r="E14" s="96"/>
-      <c r="F14" s="96"/>
-      <c r="G14" s="96"/>
-      <c r="H14" s="96"/>
-      <c r="I14" s="96"/>
-      <c r="K14" s="96" t="s">
+      <c r="B14" s="97"/>
+      <c r="C14" s="97"/>
+      <c r="D14" s="97"/>
+      <c r="E14" s="97"/>
+      <c r="F14" s="97"/>
+      <c r="G14" s="97"/>
+      <c r="H14" s="97"/>
+      <c r="I14" s="97"/>
+      <c r="K14" s="97" t="s">
         <v>271</v>
       </c>
-      <c r="L14" s="96"/>
+      <c r="L14" s="97"/>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="2" t="s">
@@ -36222,12 +36231,12 @@
     </row>
     <row r="27" spans="1:12" ht="19.5" thickBot="1"/>
     <row r="28" spans="1:12">
-      <c r="A28" s="104" t="s">
+      <c r="A28" s="105" t="s">
         <v>301</v>
       </c>
-      <c r="B28" s="105"/>
-      <c r="C28" s="105"/>
-      <c r="D28" s="105"/>
+      <c r="B28" s="106"/>
+      <c r="C28" s="106"/>
+      <c r="D28" s="106"/>
       <c r="E28" s="18">
         <f>DCOUNT(請求金額一覧表9,C15,G28:G29)</f>
         <v>4</v>
@@ -36240,12 +36249,12 @@
       </c>
     </row>
     <row r="29" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A29" s="106" t="s">
+      <c r="A29" s="107" t="s">
         <v>302</v>
       </c>
-      <c r="B29" s="107"/>
-      <c r="C29" s="107"/>
-      <c r="D29" s="107"/>
+      <c r="B29" s="108"/>
+      <c r="C29" s="108"/>
+      <c r="D29" s="108"/>
       <c r="E29" s="14">
         <f>DSUM(請求金額一覧表9,H15,I28:I29)</f>
         <v>122993</v>
@@ -36303,22 +36312,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19.5" thickBot="1">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="97" t="s">
         <v>278</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="J1" s="96" t="s">
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="J1" s="97" t="s">
         <v>300</v>
       </c>
-      <c r="K1" s="96"/>
-      <c r="L1" s="96"/>
-      <c r="M1" s="96"/>
+      <c r="K1" s="97"/>
+      <c r="L1" s="97"/>
+      <c r="M1" s="97"/>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="2" t="s">
@@ -36678,21 +36687,21 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="19.5" thickBot="1">
-      <c r="A14" s="96" t="s">
+      <c r="A14" s="97" t="s">
         <v>283</v>
       </c>
-      <c r="B14" s="96"/>
-      <c r="C14" s="96"/>
-      <c r="D14" s="96"/>
-      <c r="E14" s="96"/>
-      <c r="F14" s="96"/>
-      <c r="G14" s="96"/>
-      <c r="H14" s="96"/>
-      <c r="I14" s="96"/>
-      <c r="K14" s="96" t="s">
+      <c r="B14" s="97"/>
+      <c r="C14" s="97"/>
+      <c r="D14" s="97"/>
+      <c r="E14" s="97"/>
+      <c r="F14" s="97"/>
+      <c r="G14" s="97"/>
+      <c r="H14" s="97"/>
+      <c r="I14" s="97"/>
+      <c r="K14" s="97" t="s">
         <v>271</v>
       </c>
-      <c r="L14" s="96"/>
+      <c r="L14" s="97"/>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="2" t="s">
@@ -37076,12 +37085,12 @@
     </row>
     <row r="27" spans="1:12" ht="19.5" thickBot="1"/>
     <row r="28" spans="1:12">
-      <c r="A28" s="104" t="s">
+      <c r="A28" s="105" t="s">
         <v>301</v>
       </c>
-      <c r="B28" s="105"/>
-      <c r="C28" s="105"/>
-      <c r="D28" s="105"/>
+      <c r="B28" s="106"/>
+      <c r="C28" s="106"/>
+      <c r="D28" s="106"/>
       <c r="E28" s="18">
         <f>DCOUNT(請求金額一覧表9,C15,G28:G29)</f>
         <v>4</v>
@@ -37094,12 +37103,12 @@
       </c>
     </row>
     <row r="29" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A29" s="106" t="s">
+      <c r="A29" s="107" t="s">
         <v>302</v>
       </c>
-      <c r="B29" s="107"/>
-      <c r="C29" s="107"/>
-      <c r="D29" s="107"/>
+      <c r="B29" s="108"/>
+      <c r="C29" s="108"/>
+      <c r="D29" s="108"/>
       <c r="E29" s="14">
         <f>DSUM(請求金額一覧表9,H15,I28:I29)</f>
         <v>122993</v>
@@ -37150,23 +37159,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19.5" thickBot="1">
-      <c r="A1" s="108" t="s">
+      <c r="A1" s="109" t="s">
         <v>307</v>
       </c>
-      <c r="B1" s="108"/>
-      <c r="C1" s="108"/>
-      <c r="D1" s="108"/>
-      <c r="E1" s="108"/>
-      <c r="F1" s="108"/>
-      <c r="G1" s="108"/>
-      <c r="H1" s="108"/>
-      <c r="I1" s="108"/>
+      <c r="B1" s="109"/>
+      <c r="C1" s="109"/>
+      <c r="D1" s="109"/>
+      <c r="E1" s="109"/>
+      <c r="F1" s="109"/>
+      <c r="G1" s="109"/>
+      <c r="H1" s="109"/>
+      <c r="I1" s="109"/>
       <c r="J1" s="84"/>
-      <c r="K1" s="97" t="s">
+      <c r="K1" s="98" t="s">
         <v>321</v>
       </c>
-      <c r="L1" s="97"/>
-      <c r="M1" s="97"/>
+      <c r="L1" s="98"/>
+      <c r="M1" s="98"/>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="81" t="s">
@@ -37542,21 +37551,21 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="19.5" thickBot="1">
-      <c r="A14" s="96" t="s">
+      <c r="A14" s="97" t="s">
         <v>267</v>
       </c>
-      <c r="B14" s="96"/>
-      <c r="C14" s="96"/>
-      <c r="D14" s="96"/>
-      <c r="E14" s="96"/>
-      <c r="F14" s="96"/>
-      <c r="G14" s="96"/>
-      <c r="H14" s="96"/>
-      <c r="I14" s="96"/>
-      <c r="K14" s="96" t="s">
+      <c r="B14" s="97"/>
+      <c r="C14" s="97"/>
+      <c r="D14" s="97"/>
+      <c r="E14" s="97"/>
+      <c r="F14" s="97"/>
+      <c r="G14" s="97"/>
+      <c r="H14" s="97"/>
+      <c r="I14" s="97"/>
+      <c r="K14" s="97" t="s">
         <v>337</v>
       </c>
-      <c r="L14" s="96"/>
+      <c r="L14" s="97"/>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="81" t="s">
@@ -37940,12 +37949,12 @@
     </row>
     <row r="27" spans="1:12" ht="19.5" thickBot="1"/>
     <row r="28" spans="1:12">
-      <c r="A28" s="104" t="s">
+      <c r="A28" s="105" t="s">
         <v>338</v>
       </c>
-      <c r="B28" s="105"/>
-      <c r="C28" s="105"/>
-      <c r="D28" s="105"/>
+      <c r="B28" s="106"/>
+      <c r="C28" s="106"/>
+      <c r="D28" s="106"/>
       <c r="E28" s="69">
         <f>DSUM(請求額一覧表10,E15,K28:K29)</f>
         <v>75279</v>
@@ -37958,12 +37967,12 @@
       </c>
     </row>
     <row r="29" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A29" s="106" t="s">
+      <c r="A29" s="107" t="s">
         <v>339</v>
       </c>
-      <c r="B29" s="107"/>
-      <c r="C29" s="107"/>
-      <c r="D29" s="107"/>
+      <c r="B29" s="108"/>
+      <c r="C29" s="108"/>
+      <c r="D29" s="108"/>
       <c r="E29" s="14">
         <f>DMAX(請求額一覧表10,H15,L28:L29)</f>
         <v>76655</v>
@@ -38002,7 +38011,7 @@
   <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView showFormulas="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -38019,16 +38028,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19.5" thickBot="1">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="97" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
     </row>
     <row r="2" spans="1:11" ht="19.5" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -38055,10 +38064,10 @@
       <c r="H2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="97" t="s">
+      <c r="J2" s="98" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="97"/>
+      <c r="K2" s="98"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="5">
@@ -38241,19 +38250,19 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="19.5" thickBot="1">
-      <c r="A10" s="96" t="s">
+      <c r="A10" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="96"/>
-      <c r="C10" s="96"/>
-      <c r="D10" s="96"/>
-      <c r="E10" s="96"/>
-      <c r="F10" s="96"/>
-      <c r="G10" s="96"/>
-      <c r="H10" s="96"/>
-      <c r="I10" s="96"/>
-      <c r="J10" s="96"/>
-      <c r="K10" s="96"/>
+      <c r="B10" s="97"/>
+      <c r="C10" s="97"/>
+      <c r="D10" s="97"/>
+      <c r="E10" s="97"/>
+      <c r="F10" s="97"/>
+      <c r="G10" s="97"/>
+      <c r="H10" s="97"/>
+      <c r="I10" s="97"/>
+      <c r="J10" s="97"/>
+      <c r="K10" s="97"/>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="2" t="s">
@@ -38835,11 +38844,11 @@
       <c r="K25" s="10"/>
     </row>
     <row r="27" spans="1:11" ht="19.5" thickBot="1">
-      <c r="A27" s="97" t="s">
+      <c r="A27" s="98" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="97"/>
-      <c r="C27" s="97"/>
+      <c r="B27" s="98"/>
+      <c r="C27" s="98"/>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="2" t="s">
@@ -38949,23 +38958,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19.5" thickBot="1">
-      <c r="A1" s="108" t="s">
+      <c r="A1" s="109" t="s">
         <v>307</v>
       </c>
-      <c r="B1" s="108"/>
-      <c r="C1" s="108"/>
-      <c r="D1" s="108"/>
-      <c r="E1" s="108"/>
-      <c r="F1" s="108"/>
-      <c r="G1" s="108"/>
-      <c r="H1" s="108"/>
-      <c r="I1" s="108"/>
+      <c r="B1" s="109"/>
+      <c r="C1" s="109"/>
+      <c r="D1" s="109"/>
+      <c r="E1" s="109"/>
+      <c r="F1" s="109"/>
+      <c r="G1" s="109"/>
+      <c r="H1" s="109"/>
+      <c r="I1" s="109"/>
       <c r="J1" s="84"/>
-      <c r="K1" s="97" t="s">
+      <c r="K1" s="98" t="s">
         <v>321</v>
       </c>
-      <c r="L1" s="97"/>
-      <c r="M1" s="97"/>
+      <c r="L1" s="98"/>
+      <c r="M1" s="98"/>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="81" t="s">
@@ -39341,21 +39350,21 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="19.5" thickBot="1">
-      <c r="A14" s="96" t="s">
+      <c r="A14" s="97" t="s">
         <v>267</v>
       </c>
-      <c r="B14" s="96"/>
-      <c r="C14" s="96"/>
-      <c r="D14" s="96"/>
-      <c r="E14" s="96"/>
-      <c r="F14" s="96"/>
-      <c r="G14" s="96"/>
-      <c r="H14" s="96"/>
-      <c r="I14" s="96"/>
-      <c r="K14" s="96" t="s">
+      <c r="B14" s="97"/>
+      <c r="C14" s="97"/>
+      <c r="D14" s="97"/>
+      <c r="E14" s="97"/>
+      <c r="F14" s="97"/>
+      <c r="G14" s="97"/>
+      <c r="H14" s="97"/>
+      <c r="I14" s="97"/>
+      <c r="K14" s="97" t="s">
         <v>337</v>
       </c>
-      <c r="L14" s="96"/>
+      <c r="L14" s="97"/>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="81" t="s">
@@ -39739,12 +39748,12 @@
     </row>
     <row r="27" spans="1:12" ht="19.5" thickBot="1"/>
     <row r="28" spans="1:12">
-      <c r="A28" s="104" t="s">
+      <c r="A28" s="105" t="s">
         <v>338</v>
       </c>
-      <c r="B28" s="105"/>
-      <c r="C28" s="105"/>
-      <c r="D28" s="105"/>
+      <c r="B28" s="106"/>
+      <c r="C28" s="106"/>
+      <c r="D28" s="106"/>
       <c r="E28" s="69">
         <f>DSUM(請求額一覧表10,E15,K28:K29)</f>
         <v>75279</v>
@@ -39757,12 +39766,12 @@
       </c>
     </row>
     <row r="29" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A29" s="106" t="s">
+      <c r="A29" s="107" t="s">
         <v>339</v>
       </c>
-      <c r="B29" s="107"/>
-      <c r="C29" s="107"/>
-      <c r="D29" s="107"/>
+      <c r="B29" s="108"/>
+      <c r="C29" s="108"/>
+      <c r="D29" s="108"/>
       <c r="E29" s="14">
         <f>DMAX(請求額一覧表10,H15,L28:L29)</f>
         <v>76655</v>
@@ -39816,15 +39825,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19.5" thickBot="1">
-      <c r="A1" s="108" t="s">
+      <c r="A1" s="109" t="s">
         <v>343</v>
       </c>
-      <c r="B1" s="108"/>
-      <c r="C1" s="108"/>
-      <c r="D1" s="108"/>
-      <c r="E1" s="108"/>
-      <c r="F1" s="108"/>
-      <c r="G1" s="108"/>
+      <c r="B1" s="109"/>
+      <c r="C1" s="109"/>
+      <c r="D1" s="109"/>
+      <c r="E1" s="109"/>
+      <c r="F1" s="109"/>
+      <c r="G1" s="109"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="81" t="s">
@@ -39954,19 +39963,19 @@
       <c r="G7" s="10"/>
     </row>
     <row r="9" spans="1:11" ht="19.5" thickBot="1">
-      <c r="A9" s="96" t="s">
+      <c r="A9" s="97" t="s">
         <v>355</v>
       </c>
-      <c r="B9" s="96"/>
-      <c r="C9" s="96"/>
-      <c r="D9" s="96"/>
-      <c r="E9" s="96"/>
-      <c r="F9" s="96"/>
-      <c r="G9" s="96"/>
-      <c r="H9" s="96"/>
-      <c r="I9" s="96"/>
-      <c r="J9" s="96"/>
-      <c r="K9" s="96"/>
+      <c r="B9" s="97"/>
+      <c r="C9" s="97"/>
+      <c r="D9" s="97"/>
+      <c r="E9" s="97"/>
+      <c r="F9" s="97"/>
+      <c r="G9" s="97"/>
+      <c r="H9" s="97"/>
+      <c r="I9" s="97"/>
+      <c r="J9" s="97"/>
+      <c r="K9" s="97"/>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="81" t="s">
@@ -40422,11 +40431,11 @@
       </c>
     </row>
     <row r="23" spans="1:11" ht="19.5" thickBot="1">
-      <c r="A23" s="96" t="s">
+      <c r="A23" s="97" t="s">
         <v>375</v>
       </c>
-      <c r="B23" s="96"/>
-      <c r="C23" s="96"/>
+      <c r="B23" s="97"/>
+      <c r="C23" s="97"/>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="81" t="s">
@@ -40519,8 +40528,8 @@
   </sheetPr>
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView showFormulas="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView showFormulas="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -40539,15 +40548,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19.5" thickBot="1">
-      <c r="A1" s="108" t="s">
+      <c r="A1" s="109" t="s">
         <v>343</v>
       </c>
-      <c r="B1" s="108"/>
-      <c r="C1" s="108"/>
-      <c r="D1" s="108"/>
-      <c r="E1" s="108"/>
-      <c r="F1" s="108"/>
-      <c r="G1" s="108"/>
+      <c r="B1" s="109"/>
+      <c r="C1" s="109"/>
+      <c r="D1" s="109"/>
+      <c r="E1" s="109"/>
+      <c r="F1" s="109"/>
+      <c r="G1" s="109"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="81" t="s">
@@ -40677,19 +40686,19 @@
       <c r="G7" s="10"/>
     </row>
     <row r="9" spans="1:11" ht="19.5" thickBot="1">
-      <c r="A9" s="96" t="s">
+      <c r="A9" s="97" t="s">
         <v>355</v>
       </c>
-      <c r="B9" s="96"/>
-      <c r="C9" s="96"/>
-      <c r="D9" s="96"/>
-      <c r="E9" s="96"/>
-      <c r="F9" s="96"/>
-      <c r="G9" s="96"/>
-      <c r="H9" s="96"/>
-      <c r="I9" s="96"/>
-      <c r="J9" s="96"/>
-      <c r="K9" s="96"/>
+      <c r="B9" s="97"/>
+      <c r="C9" s="97"/>
+      <c r="D9" s="97"/>
+      <c r="E9" s="97"/>
+      <c r="F9" s="97"/>
+      <c r="G9" s="97"/>
+      <c r="H9" s="97"/>
+      <c r="I9" s="97"/>
+      <c r="J9" s="97"/>
+      <c r="K9" s="97"/>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="81" t="s">
@@ -41145,11 +41154,11 @@
       </c>
     </row>
     <row r="23" spans="1:11" ht="19.5" thickBot="1">
-      <c r="A23" s="96" t="s">
+      <c r="A23" s="97" t="s">
         <v>375</v>
       </c>
-      <c r="B23" s="96"/>
-      <c r="C23" s="96"/>
+      <c r="B23" s="97"/>
+      <c r="C23" s="97"/>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="81" t="s">
@@ -41257,20 +41266,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19.5" thickBot="1">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="97" t="s">
         <v>378</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="I1" s="114" t="s">
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="I1" s="115" t="s">
         <v>396</v>
       </c>
-      <c r="J1" s="114"/>
-      <c r="K1" s="114"/>
+      <c r="J1" s="115"/>
+      <c r="K1" s="115"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="81" t="s">
@@ -41539,10 +41548,10 @@
         <f t="shared" si="1"/>
         <v>0.93600000000000005</v>
       </c>
-      <c r="I10" s="96" t="s">
+      <c r="I10" s="97" t="s">
         <v>411</v>
       </c>
-      <c r="J10" s="96"/>
+      <c r="J10" s="97"/>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="5"/>
@@ -41577,18 +41586,18 @@
       <c r="G12" s="10"/>
     </row>
     <row r="14" spans="1:11" ht="19.5" thickBot="1">
-      <c r="A14" s="96" t="s">
+      <c r="A14" s="97" t="s">
         <v>401</v>
       </c>
-      <c r="B14" s="96"/>
-      <c r="C14" s="96"/>
-      <c r="D14" s="96"/>
-      <c r="E14" s="96"/>
-      <c r="F14" s="96"/>
-      <c r="G14" s="96"/>
-      <c r="H14" s="96"/>
-      <c r="I14" s="96"/>
-      <c r="J14" s="96"/>
+      <c r="B14" s="97"/>
+      <c r="C14" s="97"/>
+      <c r="D14" s="97"/>
+      <c r="E14" s="97"/>
+      <c r="F14" s="97"/>
+      <c r="G14" s="97"/>
+      <c r="H14" s="97"/>
+      <c r="I14" s="97"/>
+      <c r="J14" s="97"/>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="81" t="s">
@@ -41993,12 +42002,12 @@
     </row>
     <row r="27" spans="1:10" ht="19.5" thickBot="1"/>
     <row r="28" spans="1:10">
-      <c r="A28" s="104" t="s">
+      <c r="A28" s="105" t="s">
         <v>408</v>
       </c>
-      <c r="B28" s="105"/>
-      <c r="C28" s="105"/>
-      <c r="D28" s="105"/>
+      <c r="B28" s="106"/>
+      <c r="C28" s="106"/>
+      <c r="D28" s="106"/>
       <c r="E28" s="69">
         <f>DMIN(発注先別支払額一覧表12,H15,I28:I29)</f>
         <v>426955</v>
@@ -42011,12 +42020,12 @@
       </c>
     </row>
     <row r="29" spans="1:10" ht="19.5" thickBot="1">
-      <c r="A29" s="106" t="s">
+      <c r="A29" s="107" t="s">
         <v>409</v>
       </c>
-      <c r="B29" s="107"/>
-      <c r="C29" s="107"/>
-      <c r="D29" s="107"/>
+      <c r="B29" s="108"/>
+      <c r="C29" s="108"/>
+      <c r="D29" s="108"/>
       <c r="E29" s="14">
         <f>ROUND(DAVERAGE(発注先別支払額一覧表12,G15,J28:J29),0)</f>
         <v>21406</v>
@@ -42054,8 +42063,8 @@
   </sheetPr>
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView showFormulas="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView showFormulas="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -42072,20 +42081,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19.5" thickBot="1">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="97" t="s">
         <v>378</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="I1" s="114" t="s">
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="I1" s="115" t="s">
         <v>396</v>
       </c>
-      <c r="J1" s="114"/>
-      <c r="K1" s="114"/>
+      <c r="J1" s="115"/>
+      <c r="K1" s="115"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="81" t="s">
@@ -42354,10 +42363,10 @@
         <f t="shared" si="1"/>
         <v>0.93600000000000005</v>
       </c>
-      <c r="I10" s="96" t="s">
+      <c r="I10" s="97" t="s">
         <v>411</v>
       </c>
-      <c r="J10" s="96"/>
+      <c r="J10" s="97"/>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="5"/>
@@ -42392,18 +42401,18 @@
       <c r="G12" s="10"/>
     </row>
     <row r="14" spans="1:11" ht="19.5" thickBot="1">
-      <c r="A14" s="96" t="s">
+      <c r="A14" s="97" t="s">
         <v>401</v>
       </c>
-      <c r="B14" s="96"/>
-      <c r="C14" s="96"/>
-      <c r="D14" s="96"/>
-      <c r="E14" s="96"/>
-      <c r="F14" s="96"/>
-      <c r="G14" s="96"/>
-      <c r="H14" s="96"/>
-      <c r="I14" s="96"/>
-      <c r="J14" s="96"/>
+      <c r="B14" s="97"/>
+      <c r="C14" s="97"/>
+      <c r="D14" s="97"/>
+      <c r="E14" s="97"/>
+      <c r="F14" s="97"/>
+      <c r="G14" s="97"/>
+      <c r="H14" s="97"/>
+      <c r="I14" s="97"/>
+      <c r="J14" s="97"/>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="81" t="s">
@@ -42808,12 +42817,12 @@
     </row>
     <row r="27" spans="1:10" ht="19.5" thickBot="1"/>
     <row r="28" spans="1:10">
-      <c r="A28" s="104" t="s">
+      <c r="A28" s="105" t="s">
         <v>408</v>
       </c>
-      <c r="B28" s="105"/>
-      <c r="C28" s="105"/>
-      <c r="D28" s="105"/>
+      <c r="B28" s="106"/>
+      <c r="C28" s="106"/>
+      <c r="D28" s="106"/>
       <c r="E28" s="69">
         <f>DMIN(発注先別支払額一覧表12,H15,I28:I29)</f>
         <v>426955</v>
@@ -42826,12 +42835,12 @@
       </c>
     </row>
     <row r="29" spans="1:10" ht="19.5" thickBot="1">
-      <c r="A29" s="106" t="s">
+      <c r="A29" s="107" t="s">
         <v>409</v>
       </c>
-      <c r="B29" s="107"/>
-      <c r="C29" s="107"/>
-      <c r="D29" s="107"/>
+      <c r="B29" s="108"/>
+      <c r="C29" s="108"/>
+      <c r="D29" s="108"/>
       <c r="E29" s="14">
         <f>ROUND(DAVERAGE(発注先別支払額一覧表12,G15,J28:J29),0)</f>
         <v>21406</v>
@@ -42862,12 +42871,13 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCF515CC-AEDA-4AAD-B2CB-8F022A0BE6C5}">
   <sheetPr>
+    <tabColor rgb="FFFF0000"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -42886,21 +42896,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="19.5" thickBot="1">
-      <c r="A1" s="98" t="s">
+      <c r="A1" s="99" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="98"/>
-      <c r="H1" s="98"/>
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="99"/>
+      <c r="E1" s="99"/>
+      <c r="F1" s="99"/>
+      <c r="G1" s="99"/>
+      <c r="H1" s="99"/>
       <c r="I1" s="19"/>
-      <c r="J1" s="98" t="s">
+      <c r="J1" s="99" t="s">
         <v>39</v>
       </c>
-      <c r="K1" s="98"/>
+      <c r="K1" s="99"/>
       <c r="L1" s="19"/>
     </row>
     <row r="2" spans="1:14">
@@ -43081,10 +43091,10 @@
         <v>3500</v>
       </c>
       <c r="I6" s="19"/>
-      <c r="J6" s="99" t="s">
+      <c r="J6" s="100" t="s">
         <v>57</v>
       </c>
-      <c r="K6" s="99"/>
+      <c r="K6" s="100"/>
       <c r="L6" s="19"/>
     </row>
     <row r="7" spans="1:14">
@@ -43171,19 +43181,19 @@
       <c r="L10" s="19"/>
     </row>
     <row r="11" spans="1:14" ht="19.5" thickBot="1">
-      <c r="A11" s="98" t="s">
+      <c r="A11" s="99" t="s">
         <v>61</v>
       </c>
-      <c r="B11" s="98"/>
-      <c r="C11" s="98"/>
-      <c r="D11" s="98"/>
-      <c r="E11" s="98"/>
-      <c r="F11" s="98"/>
-      <c r="G11" s="98"/>
-      <c r="H11" s="98"/>
-      <c r="I11" s="98"/>
-      <c r="J11" s="98"/>
-      <c r="K11" s="98"/>
+      <c r="B11" s="99"/>
+      <c r="C11" s="99"/>
+      <c r="D11" s="99"/>
+      <c r="E11" s="99"/>
+      <c r="F11" s="99"/>
+      <c r="G11" s="99"/>
+      <c r="H11" s="99"/>
+      <c r="I11" s="99"/>
+      <c r="J11" s="99"/>
+      <c r="K11" s="99"/>
       <c r="L11" s="19"/>
     </row>
     <row r="12" spans="1:14">
@@ -43840,11 +43850,11 @@
       <c r="N27" s="19"/>
     </row>
     <row r="28" spans="1:14" ht="19.5" thickBot="1">
-      <c r="A28" s="98" t="s">
+      <c r="A28" s="99" t="s">
         <v>68</v>
       </c>
-      <c r="B28" s="98"/>
-      <c r="C28" s="98"/>
+      <c r="B28" s="99"/>
+      <c r="C28" s="99"/>
       <c r="D28" s="19"/>
       <c r="E28" s="19"/>
       <c r="F28" s="19"/>
@@ -43858,13 +43868,13 @@
       <c r="N28" s="19"/>
     </row>
     <row r="29" spans="1:14">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="94" t="s">
         <v>49</v>
       </c>
-      <c r="B29" s="40" t="s">
+      <c r="B29" s="95" t="s">
         <v>63</v>
       </c>
-      <c r="C29" s="41" t="s">
+      <c r="C29" s="96" t="s">
         <v>66</v>
       </c>
       <c r="D29" s="19"/>
@@ -43999,7 +44009,7 @@
   </sheetPr>
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView showFormulas="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView showFormulas="1" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -44021,21 +44031,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="19.5" thickBot="1">
-      <c r="A1" s="98" t="s">
+      <c r="A1" s="99" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="98"/>
-      <c r="H1" s="98"/>
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="99"/>
+      <c r="E1" s="99"/>
+      <c r="F1" s="99"/>
+      <c r="G1" s="99"/>
+      <c r="H1" s="99"/>
       <c r="I1" s="19"/>
-      <c r="J1" s="98" t="s">
+      <c r="J1" s="99" t="s">
         <v>39</v>
       </c>
-      <c r="K1" s="98"/>
+      <c r="K1" s="99"/>
       <c r="L1" s="19"/>
     </row>
     <row r="2" spans="1:14">
@@ -44216,10 +44226,10 @@
         <v>3500</v>
       </c>
       <c r="I6" s="19"/>
-      <c r="J6" s="99" t="s">
+      <c r="J6" s="100" t="s">
         <v>57</v>
       </c>
-      <c r="K6" s="99"/>
+      <c r="K6" s="100"/>
       <c r="L6" s="19"/>
     </row>
     <row r="7" spans="1:14">
@@ -44306,19 +44316,19 @@
       <c r="L10" s="19"/>
     </row>
     <row r="11" spans="1:14" ht="19.5" thickBot="1">
-      <c r="A11" s="98" t="s">
+      <c r="A11" s="99" t="s">
         <v>61</v>
       </c>
-      <c r="B11" s="98"/>
-      <c r="C11" s="98"/>
-      <c r="D11" s="98"/>
-      <c r="E11" s="98"/>
-      <c r="F11" s="98"/>
-      <c r="G11" s="98"/>
-      <c r="H11" s="98"/>
-      <c r="I11" s="98"/>
-      <c r="J11" s="98"/>
-      <c r="K11" s="98"/>
+      <c r="B11" s="99"/>
+      <c r="C11" s="99"/>
+      <c r="D11" s="99"/>
+      <c r="E11" s="99"/>
+      <c r="F11" s="99"/>
+      <c r="G11" s="99"/>
+      <c r="H11" s="99"/>
+      <c r="I11" s="99"/>
+      <c r="J11" s="99"/>
+      <c r="K11" s="99"/>
       <c r="L11" s="19"/>
     </row>
     <row r="12" spans="1:14">
@@ -44975,11 +44985,11 @@
       <c r="N27" s="19"/>
     </row>
     <row r="28" spans="1:14" ht="19.5" thickBot="1">
-      <c r="A28" s="98" t="s">
+      <c r="A28" s="99" t="s">
         <v>68</v>
       </c>
-      <c r="B28" s="98"/>
-      <c r="C28" s="98"/>
+      <c r="B28" s="99"/>
+      <c r="C28" s="99"/>
       <c r="D28" s="19"/>
       <c r="E28" s="19"/>
       <c r="F28" s="19"/>
@@ -45134,8 +45144,8 @@
   </sheetPr>
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -45148,13 +45158,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="97" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="2" t="s">
@@ -45250,56 +45260,56 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A8" s="96" t="s">
+      <c r="A8" s="97" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="96"/>
-      <c r="C8" s="96"/>
-      <c r="D8" s="96"/>
-      <c r="E8" s="96"/>
-      <c r="F8" s="96"/>
-      <c r="G8" s="96"/>
-      <c r="H8" s="96"/>
-      <c r="I8" s="96"/>
-      <c r="J8" s="96"/>
-      <c r="K8" s="96"/>
-      <c r="L8" s="96"/>
+      <c r="B8" s="97"/>
+      <c r="C8" s="97"/>
+      <c r="D8" s="97"/>
+      <c r="E8" s="97"/>
+      <c r="F8" s="97"/>
+      <c r="G8" s="97"/>
+      <c r="H8" s="97"/>
+      <c r="I8" s="97"/>
+      <c r="J8" s="97"/>
+      <c r="K8" s="97"/>
+      <c r="L8" s="97"/>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="94" t="s">
+      <c r="A9" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B9" s="95" t="s">
+      <c r="B9" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C9" s="95" t="s">
+      <c r="C9" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D9" s="95" t="s">
+      <c r="D9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="95" t="s">
+      <c r="E9" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="F9" s="95" t="s">
+      <c r="F9" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="G9" s="95" t="s">
+      <c r="G9" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="H9" s="95" t="s">
+      <c r="H9" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="I9" s="95" t="s">
+      <c r="I9" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="J9" s="95" t="s">
+      <c r="J9" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="K9" s="21" t="s">
+      <c r="K9" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="L9" s="22" t="s">
+      <c r="L9" s="41" t="s">
         <v>97</v>
       </c>
     </row>
@@ -45724,12 +45734,12 @@
     </row>
     <row r="21" spans="1:12" ht="19.5" thickBot="1"/>
     <row r="22" spans="1:12">
-      <c r="A22" s="102" t="s">
+      <c r="A22" s="103" t="s">
         <v>98</v>
       </c>
-      <c r="B22" s="103"/>
-      <c r="C22" s="103"/>
-      <c r="D22" s="103"/>
+      <c r="B22" s="104"/>
+      <c r="C22" s="104"/>
+      <c r="D22" s="104"/>
       <c r="E22" s="18">
         <f>DCOUNT(請求金額一覧表3,11,$G$22:$G$23)</f>
         <v>5</v>
@@ -45739,12 +45749,12 @@
       </c>
     </row>
     <row r="23" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A23" s="100" t="s">
+      <c r="A23" s="101" t="s">
         <v>99</v>
       </c>
-      <c r="B23" s="101"/>
-      <c r="C23" s="101"/>
-      <c r="D23" s="101"/>
+      <c r="B23" s="102"/>
+      <c r="C23" s="102"/>
+      <c r="D23" s="102"/>
       <c r="E23" s="14">
         <f>DSUM(請求金額一覧表3,9,G24:G25)</f>
         <v>525610</v>
@@ -45788,7 +45798,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView showFormulas="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:D22"/>
+      <selection activeCell="A2" sqref="A1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -45808,13 +45818,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="97" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="2" t="s">
@@ -45910,20 +45920,20 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A8" s="96" t="s">
+      <c r="A8" s="97" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="96"/>
-      <c r="C8" s="96"/>
-      <c r="D8" s="96"/>
-      <c r="E8" s="96"/>
-      <c r="F8" s="96"/>
-      <c r="G8" s="96"/>
-      <c r="H8" s="96"/>
-      <c r="I8" s="96"/>
-      <c r="J8" s="96"/>
-      <c r="K8" s="96"/>
-      <c r="L8" s="96"/>
+      <c r="B8" s="97"/>
+      <c r="C8" s="97"/>
+      <c r="D8" s="97"/>
+      <c r="E8" s="97"/>
+      <c r="F8" s="97"/>
+      <c r="G8" s="97"/>
+      <c r="H8" s="97"/>
+      <c r="I8" s="97"/>
+      <c r="J8" s="97"/>
+      <c r="K8" s="97"/>
+      <c r="L8" s="97"/>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="2" t="s">
@@ -46384,12 +46394,12 @@
     </row>
     <row r="21" spans="1:12" ht="19.5" thickBot="1"/>
     <row r="22" spans="1:12">
-      <c r="A22" s="102" t="s">
+      <c r="A22" s="103" t="s">
         <v>98</v>
       </c>
-      <c r="B22" s="103"/>
-      <c r="C22" s="103"/>
-      <c r="D22" s="103"/>
+      <c r="B22" s="104"/>
+      <c r="C22" s="104"/>
+      <c r="D22" s="104"/>
       <c r="E22" s="18">
         <f>DCOUNT(請求金額一覧表3,11,$G$22:$G$23)</f>
         <v>5</v>
@@ -46399,12 +46409,12 @@
       </c>
     </row>
     <row r="23" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A23" s="100" t="s">
+      <c r="A23" s="101" t="s">
         <v>99</v>
       </c>
-      <c r="B23" s="101"/>
-      <c r="C23" s="101"/>
-      <c r="D23" s="101"/>
+      <c r="B23" s="102"/>
+      <c r="C23" s="102"/>
+      <c r="D23" s="102"/>
       <c r="E23" s="14">
         <f>DSUM(請求金額一覧表3,9,G24:G25)</f>
         <v>525610</v>
@@ -46463,14 +46473,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A1" s="108" t="s">
+      <c r="A1" s="109" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="108"/>
-      <c r="C1" s="108"/>
-      <c r="D1" s="108"/>
-      <c r="E1" s="108"/>
-      <c r="F1" s="108"/>
+      <c r="B1" s="109"/>
+      <c r="C1" s="109"/>
+      <c r="D1" s="109"/>
+      <c r="E1" s="109"/>
+      <c r="F1" s="109"/>
     </row>
     <row r="2" spans="1:12" ht="19.5" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -46491,14 +46501,14 @@
       <c r="F2" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="H2" s="96" t="s">
+      <c r="H2" s="97" t="s">
         <v>134</v>
       </c>
-      <c r="I2" s="96"/>
-      <c r="K2" s="97" t="s">
+      <c r="I2" s="97"/>
+      <c r="K2" s="98" t="s">
         <v>135</v>
       </c>
-      <c r="L2" s="97"/>
+      <c r="L2" s="98"/>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="5">
@@ -46637,20 +46647,20 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A8" s="96" t="s">
+      <c r="A8" s="97" t="s">
         <v>115</v>
       </c>
-      <c r="B8" s="96"/>
-      <c r="C8" s="96"/>
-      <c r="D8" s="96"/>
-      <c r="E8" s="96"/>
-      <c r="F8" s="96"/>
-      <c r="G8" s="96"/>
-      <c r="H8" s="96"/>
-      <c r="I8" s="96"/>
-      <c r="J8" s="96"/>
-      <c r="K8" s="96"/>
-      <c r="L8" s="96"/>
+      <c r="B8" s="97"/>
+      <c r="C8" s="97"/>
+      <c r="D8" s="97"/>
+      <c r="E8" s="97"/>
+      <c r="F8" s="97"/>
+      <c r="G8" s="97"/>
+      <c r="H8" s="97"/>
+      <c r="I8" s="97"/>
+      <c r="J8" s="97"/>
+      <c r="K8" s="97"/>
+      <c r="L8" s="97"/>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="2" t="s">
@@ -47100,12 +47110,12 @@
     </row>
     <row r="21" spans="1:12" ht="19.5" thickBot="1"/>
     <row r="22" spans="1:12">
-      <c r="B22" s="104" t="s">
+      <c r="B22" s="105" t="s">
         <v>143</v>
       </c>
-      <c r="C22" s="105"/>
-      <c r="D22" s="105"/>
-      <c r="E22" s="105"/>
+      <c r="C22" s="106"/>
+      <c r="D22" s="106"/>
+      <c r="E22" s="106"/>
       <c r="F22" s="69">
         <f>DSUM(依頼先別加工賃一覧表4,G9,$I$22:$I$23)</f>
         <v>1921898</v>
@@ -47118,12 +47128,12 @@
       </c>
     </row>
     <row r="23" spans="1:12" ht="19.5" thickBot="1">
-      <c r="B23" s="106" t="s">
+      <c r="B23" s="107" t="s">
         <v>142</v>
       </c>
-      <c r="C23" s="107"/>
-      <c r="D23" s="107"/>
-      <c r="E23" s="107"/>
+      <c r="C23" s="108"/>
+      <c r="D23" s="108"/>
+      <c r="E23" s="108"/>
       <c r="F23" s="14">
         <f>ROUND(DAVERAGE(依頼先別加工賃一覧表4,J9,$K$22:$K$23),0)</f>
         <v>455239</v>
@@ -47162,7 +47172,7 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView showFormulas="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="A2" sqref="A1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -47182,14 +47192,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A1" s="108" t="s">
+      <c r="A1" s="109" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="108"/>
-      <c r="C1" s="108"/>
-      <c r="D1" s="108"/>
-      <c r="E1" s="108"/>
-      <c r="F1" s="108"/>
+      <c r="B1" s="109"/>
+      <c r="C1" s="109"/>
+      <c r="D1" s="109"/>
+      <c r="E1" s="109"/>
+      <c r="F1" s="109"/>
     </row>
     <row r="2" spans="1:12" ht="19.5" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -47210,14 +47220,14 @@
       <c r="F2" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="H2" s="96" t="s">
+      <c r="H2" s="97" t="s">
         <v>134</v>
       </c>
-      <c r="I2" s="96"/>
-      <c r="K2" s="97" t="s">
+      <c r="I2" s="97"/>
+      <c r="K2" s="98" t="s">
         <v>135</v>
       </c>
-      <c r="L2" s="97"/>
+      <c r="L2" s="98"/>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="5">
@@ -47356,20 +47366,20 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A8" s="96" t="s">
+      <c r="A8" s="97" t="s">
         <v>115</v>
       </c>
-      <c r="B8" s="96"/>
-      <c r="C8" s="96"/>
-      <c r="D8" s="96"/>
-      <c r="E8" s="96"/>
-      <c r="F8" s="96"/>
-      <c r="G8" s="96"/>
-      <c r="H8" s="96"/>
-      <c r="I8" s="96"/>
-      <c r="J8" s="96"/>
-      <c r="K8" s="96"/>
-      <c r="L8" s="96"/>
+      <c r="B8" s="97"/>
+      <c r="C8" s="97"/>
+      <c r="D8" s="97"/>
+      <c r="E8" s="97"/>
+      <c r="F8" s="97"/>
+      <c r="G8" s="97"/>
+      <c r="H8" s="97"/>
+      <c r="I8" s="97"/>
+      <c r="J8" s="97"/>
+      <c r="K8" s="97"/>
+      <c r="L8" s="97"/>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="2" t="s">
@@ -47819,12 +47829,12 @@
     </row>
     <row r="21" spans="1:12" ht="19.5" thickBot="1"/>
     <row r="22" spans="1:12">
-      <c r="B22" s="104" t="s">
+      <c r="B22" s="105" t="s">
         <v>143</v>
       </c>
-      <c r="C22" s="105"/>
-      <c r="D22" s="105"/>
-      <c r="E22" s="105"/>
+      <c r="C22" s="106"/>
+      <c r="D22" s="106"/>
+      <c r="E22" s="106"/>
       <c r="F22" s="69">
         <f>DSUM(依頼先別加工賃一覧表4,G9,$I$22:$I$23)</f>
         <v>1921898</v>
@@ -47837,12 +47847,12 @@
       </c>
     </row>
     <row r="23" spans="1:12" ht="19.5" thickBot="1">
-      <c r="B23" s="106" t="s">
+      <c r="B23" s="107" t="s">
         <v>142</v>
       </c>
-      <c r="C23" s="107"/>
-      <c r="D23" s="107"/>
-      <c r="E23" s="107"/>
+      <c r="C23" s="108"/>
+      <c r="D23" s="108"/>
+      <c r="E23" s="108"/>
       <c r="F23" s="14">
         <f>ROUND(DAVERAGE(依頼先別加工賃一覧表4,J9,$K$22:$K$23),0)</f>
         <v>455239</v>
@@ -47893,22 +47903,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="97" t="s">
         <v>148</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="H1" s="97" t="s">
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="H1" s="98" t="s">
         <v>159</v>
       </c>
-      <c r="I1" s="97"/>
-      <c r="K1" s="97" t="s">
+      <c r="I1" s="98"/>
+      <c r="K1" s="98" t="s">
         <v>163</v>
       </c>
-      <c r="L1" s="97"/>
+      <c r="L1" s="98"/>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="2" t="s">
@@ -48073,20 +48083,20 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A8" s="96" t="s">
+      <c r="A8" s="97" t="s">
         <v>174</v>
       </c>
-      <c r="B8" s="96"/>
-      <c r="C8" s="96"/>
-      <c r="D8" s="96"/>
-      <c r="E8" s="96"/>
-      <c r="F8" s="96"/>
-      <c r="G8" s="96"/>
-      <c r="H8" s="96"/>
-      <c r="I8" s="96"/>
-      <c r="J8" s="96"/>
-      <c r="K8" s="96"/>
-      <c r="L8" s="96"/>
+      <c r="B8" s="97"/>
+      <c r="C8" s="97"/>
+      <c r="D8" s="97"/>
+      <c r="E8" s="97"/>
+      <c r="F8" s="97"/>
+      <c r="G8" s="97"/>
+      <c r="H8" s="97"/>
+      <c r="I8" s="97"/>
+      <c r="J8" s="97"/>
+      <c r="K8" s="97"/>
+      <c r="L8" s="97"/>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="2" t="s">
@@ -48761,11 +48771,11 @@
       <c r="L24" s="10"/>
     </row>
     <row r="26" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A26" s="109" t="s">
+      <c r="A26" s="110" t="s">
         <v>181</v>
       </c>
-      <c r="B26" s="109"/>
-      <c r="C26" s="109"/>
+      <c r="B26" s="110"/>
+      <c r="C26" s="110"/>
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="2" t="s">

</xml_diff>